<commit_message>
With medium res and proper checkpoints saving
</commit_message>
<xml_diff>
--- a/Convolutional network size calculator.xlsx
+++ b/Convolutional network size calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timva\Documents\GitHub\Sparse-recovery-of-IR-images-using-a-score-based-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739EE863-EFF2-4989-8C38-45FAC2AE3A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A800E130-AD9A-457B-BD15-E21344A9CBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B2DC737-34CF-420A-AF9A-B9F1BF30D588}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="29">
   <si>
     <t>Hin</t>
   </si>
@@ -322,9 +322,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -671,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E69EC-ECC9-4653-A3EC-CA67F7716823}">
-  <dimension ref="A1:AM57"/>
+  <dimension ref="A1:AM71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AO42" sqref="AO42"/>
+    <sheetView tabSelected="1" topLeftCell="W26" zoomScale="106" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40:P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,42 +706,42 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="I4" s="21" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
+      <c r="I4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="23"/>
-      <c r="Q4" s="21" t="s">
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="22"/>
+      <c r="Q4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="23"/>
-      <c r="Y4" s="21" t="s">
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="22"/>
+      <c r="Y4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="23"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="22"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -1128,64 +1128,64 @@
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="Y9" s="24" t="s">
+      <c r="Y9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="24"/>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="24"/>
-      <c r="AD9" s="24"/>
-      <c r="AE9" s="24"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="23"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="23"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Y10" s="20" t="s">
+      <c r="Y10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-      <c r="AE10" s="20"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="I11" s="21" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="I11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="23"/>
-      <c r="Q11" s="21" t="s">
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="22"/>
+      <c r="Q11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="23"/>
-      <c r="Y11" s="21" t="s">
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="22"/>
+      <c r="Y11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22"/>
-      <c r="AE11" s="23"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="21"/>
+      <c r="AE11" s="22"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1578,7 +1578,7 @@
       <c r="P16" s="8"/>
       <c r="X16" s="8"/>
     </row>
-    <row r="17" spans="1:31" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
@@ -1586,45 +1586,45 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+    <row r="18" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
-      <c r="I18" s="21" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="I18" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="23"/>
-      <c r="Q18" s="21" t="s">
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="22"/>
+      <c r="Q18" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="23"/>
-      <c r="Y18" s="21" t="s">
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="22"/>
+      <c r="Y18" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="22"/>
-      <c r="AD18" s="22"/>
-      <c r="AE18" s="23"/>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+      <c r="AB18" s="21"/>
+      <c r="AC18" s="21"/>
+      <c r="AD18" s="21"/>
+      <c r="AE18" s="22"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>0</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>128</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>6</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>160</v>
       </c>
@@ -2008,67 +2008,67 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="Y23" s="24" t="s">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="Y23" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="24"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
-      <c r="AD23" s="24"/>
-      <c r="AE23" s="24"/>
-    </row>
-    <row r="24" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Y24" s="20" t="s">
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="23"/>
+    </row>
+    <row r="24" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y24" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="Z24" s="20"/>
-      <c r="AA24" s="20"/>
-      <c r="AB24" s="20"/>
-      <c r="AC24" s="20"/>
-      <c r="AD24" s="20"/>
-      <c r="AE24" s="20"/>
-    </row>
-    <row r="25" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="24"/>
+      <c r="AB24" s="24"/>
+      <c r="AC24" s="24"/>
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="24"/>
+    </row>
+    <row r="25" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="23"/>
-      <c r="I25" s="21" t="s">
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+      <c r="I25" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="23"/>
-      <c r="Q25" s="21" t="s">
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="22"/>
+      <c r="Q25" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="22"/>
-      <c r="U25" s="22"/>
-      <c r="V25" s="22"/>
-      <c r="W25" s="23"/>
-      <c r="Y25" s="21" t="s">
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="22"/>
+      <c r="Y25" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="Z25" s="22"/>
-      <c r="AA25" s="22"/>
-      <c r="AB25" s="22"/>
-      <c r="AC25" s="22"/>
-      <c r="AD25" s="22"/>
-      <c r="AE25" s="23"/>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="21"/>
+      <c r="AB25" s="21"/>
+      <c r="AC25" s="21"/>
+      <c r="AD25" s="21"/>
+      <c r="AE25" s="22"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>O27</f>
         <v>64</v>
@@ -2264,7 +2264,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <f>O29</f>
         <v>80</v>
@@ -2454,59 +2454,68 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:31" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H30" s="8"/>
       <c r="P30" s="8"/>
       <c r="X30" s="8"/>
     </row>
-    <row r="31" spans="1:31" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="X31" s="8"/>
-    </row>
-    <row r="32" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="23"/>
-      <c r="I32" s="21" t="s">
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
+      <c r="I32" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="23"/>
-      <c r="Q32" s="21" t="s">
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="22"/>
+      <c r="Q32" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
-      <c r="U32" s="22"/>
-      <c r="V32" s="22"/>
-      <c r="W32" s="23"/>
-      <c r="Y32" s="21" t="s">
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="22"/>
+      <c r="Y32" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Z32" s="22"/>
-      <c r="AA32" s="22"/>
-      <c r="AB32" s="22"/>
-      <c r="AC32" s="22"/>
-      <c r="AD32" s="22"/>
-      <c r="AE32" s="23"/>
+      <c r="Z32" s="21"/>
+      <c r="AA32" s="21"/>
+      <c r="AB32" s="21"/>
+      <c r="AC32" s="21"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="22"/>
+      <c r="AG32" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH32" s="21"/>
+      <c r="AI32" s="21"/>
+      <c r="AJ32" s="21"/>
+      <c r="AK32" s="21"/>
+      <c r="AL32" s="21"/>
+      <c r="AM32" s="22"/>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -2575,7 +2584,7 @@
       <c r="V33" t="s">
         <v>21</v>
       </c>
-      <c r="W33" s="13" t="s">
+      <c r="W33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="X33" s="19" t="s">
@@ -2599,13 +2608,37 @@
       <c r="AD33" t="s">
         <v>21</v>
       </c>
-      <c r="AE33" s="2" t="s">
+      <c r="AE33" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF33" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM33" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2625,15 +2658,15 @@
       </c>
       <c r="G34" s="2">
         <f>(A34 + 2 * B34 - C34*(D34-1) -1) / E34 + 1</f>
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="1">
         <f>G34</f>
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -2642,20 +2675,20 @@
         <v>4</v>
       </c>
       <c r="M34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N34">
         <f>I34/O34</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O34" s="2">
         <f>((I34 + 2 * J34 - K34*(L34-1) -1) / M34 )+ 1</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="P34" s="19"/>
       <c r="Q34" s="1">
         <f>O34</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="R34">
         <v>1</v>
@@ -2664,43 +2697,68 @@
         <v>1</v>
       </c>
       <c r="T34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U34">
         <v>2</v>
       </c>
       <c r="V34">
         <f>Q34/W34</f>
-        <v>1.9393939393939394</v>
-      </c>
-      <c r="W34" s="13">
-        <f>(Q34 + 2 * R34 - S34*(T34-1) -1) / U34 + 1</f>
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="W34" s="2">
+        <f>((Q34 + 2 * R34 - S34*(T34-1) -1) / U34 )+ 1</f>
+        <v>16</v>
       </c>
       <c r="X34" s="19"/>
       <c r="Y34" s="1">
         <f>W34</f>
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="Z34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA34">
         <v>1</v>
       </c>
       <c r="AB34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC34">
         <v>2</v>
       </c>
       <c r="AD34">
         <f>Y34/AE34</f>
-        <v>2.0625</v>
-      </c>
-      <c r="AE34" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE34" s="13">
         <f>(Y34 + 2 * Z34 - AA34*(AB34-1) -1) / AC34 + 1</f>
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="AF34" s="19"/>
+      <c r="AG34" s="1">
+        <f>AE34</f>
+        <v>8</v>
+      </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <v>1</v>
+      </c>
+      <c r="AJ34">
+        <v>2</v>
+      </c>
+      <c r="AK34">
+        <v>2</v>
+      </c>
+      <c r="AL34">
+        <f>AG34/AM34</f>
+        <v>2</v>
+      </c>
+      <c r="AM34" s="2">
+        <f>(AG34 + 2 * AH34 - AI34*(AJ34-1) -1) / AK34 + 1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
@@ -2766,7 +2824,7 @@
       <c r="V35" t="s">
         <v>21</v>
       </c>
-      <c r="W35" s="13" t="s">
+      <c r="W35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="X35" s="19"/>
@@ -2788,13 +2846,35 @@
       <c r="AD35" t="s">
         <v>21</v>
       </c>
-      <c r="AE35" s="2" t="s">
+      <c r="AE35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF35" s="19"/>
+      <c r="AG35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL35" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
-        <v>640</v>
+        <v>160</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
@@ -2814,37 +2894,37 @@
       </c>
       <c r="G36" s="5">
         <f>(A36 + 2 * B36 - C36*(D36-1) -1) / E36 + 1</f>
-        <v>320</v>
+        <v>80</v>
       </c>
       <c r="H36" s="19"/>
       <c r="I36" s="3">
         <f>G36</f>
-        <v>320</v>
+        <v>80</v>
       </c>
       <c r="J36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="4">
         <v>1</v>
       </c>
       <c r="L36" s="4">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="M36" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N36" s="4">
         <f>I36/O36</f>
-        <v>4.1025641025641022</v>
+        <v>2</v>
       </c>
       <c r="O36" s="5">
         <f>(I36 + 2 * J36 - K36*(L36-1) -1) / M36 + 1</f>
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="P36" s="19"/>
       <c r="Q36" s="3">
         <f>O36</f>
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="R36" s="4">
         <v>1</v>
@@ -2853,104 +2933,138 @@
         <v>1</v>
       </c>
       <c r="T36" s="4">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="U36" s="4">
         <v>2</v>
       </c>
       <c r="V36" s="4">
         <f>Q36/W36</f>
-        <v>2.3636363636363638</v>
-      </c>
-      <c r="W36" s="14">
+        <v>2</v>
+      </c>
+      <c r="W36" s="5">
         <f>(Q36 + 2 * R36 - S36*(T36-1) -1) / U36 + 1</f>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="X36" s="19"/>
       <c r="Y36" s="3">
         <f>W36</f>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="Z36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA36" s="4">
         <v>1</v>
       </c>
       <c r="AB36" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC36" s="4">
         <v>2</v>
       </c>
       <c r="AD36" s="4">
         <f>Y36/AE36</f>
-        <v>2.0625</v>
-      </c>
-      <c r="AE36" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE36" s="14">
         <f>(Y36 + 2 * Z36 - AA36*(AB36-1) -1) / AC36 + 1</f>
+        <v>10</v>
+      </c>
+      <c r="AF36" s="19"/>
+      <c r="AG36" s="3">
+        <f>AE36</f>
+        <v>10</v>
+      </c>
+      <c r="AH36" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI36" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK36" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL36" s="4">
+        <f>AG36/AM36</f>
+        <v>2</v>
+      </c>
+      <c r="AM36" s="5">
+        <f>(AG36 + 2 * AH36 - AI36*(AJ36-1) -1) / AK36 + 1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AG37" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH37" s="23"/>
+      <c r="AI37" s="23"/>
+      <c r="AJ37" s="23"/>
+      <c r="AK37" s="23"/>
+      <c r="AL37" s="23"/>
+      <c r="AM37" s="23"/>
+    </row>
+    <row r="38" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG38" s="24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="Y37" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z37" s="24"/>
-      <c r="AA37" s="24"/>
-      <c r="AB37" s="24"/>
-      <c r="AC37" s="24"/>
-      <c r="AD37" s="24"/>
-      <c r="AE37" s="24"/>
-    </row>
-    <row r="38" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Y38" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z38" s="20"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="20"/>
-      <c r="AC38" s="20"/>
-      <c r="AD38" s="20"/>
-      <c r="AE38" s="20"/>
+      <c r="AH38" s="24"/>
+      <c r="AI38" s="24"/>
+      <c r="AJ38" s="24"/>
+      <c r="AK38" s="24"/>
+      <c r="AL38" s="24"/>
+      <c r="AM38" s="24"/>
     </row>
     <row r="39" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="23"/>
-      <c r="I39" s="21" t="s">
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="22"/>
+      <c r="I39" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="23"/>
-      <c r="Q39" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="R39" s="22"/>
-      <c r="S39" s="22"/>
-      <c r="T39" s="22"/>
-      <c r="U39" s="22"/>
-      <c r="V39" s="22"/>
-      <c r="W39" s="23"/>
-      <c r="Y39" s="21" t="s">
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="22"/>
+      <c r="Q39" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="22"/>
+      <c r="Y39" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="Z39" s="22"/>
-      <c r="AA39" s="22"/>
-      <c r="AB39" s="22"/>
-      <c r="AC39" s="22"/>
-      <c r="AD39" s="22"/>
-      <c r="AE39" s="23"/>
+      <c r="Z39" s="21"/>
+      <c r="AA39" s="21"/>
+      <c r="AB39" s="21"/>
+      <c r="AC39" s="21"/>
+      <c r="AD39" s="21"/>
+      <c r="AE39" s="22"/>
+      <c r="AG39" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH39" s="21"/>
+      <c r="AI39" s="21"/>
+      <c r="AJ39" s="21"/>
+      <c r="AK39" s="21"/>
+      <c r="AL39" s="21"/>
+      <c r="AM39" s="22"/>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -3001,7 +3115,7 @@
       <c r="P40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="Q40" s="15" t="s">
+      <c r="Q40" s="1" t="s">
         <v>0</v>
       </c>
       <c r="R40" t="s">
@@ -3025,7 +3139,7 @@
       <c r="X40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="Y40" s="1" t="s">
+      <c r="Y40" s="15" t="s">
         <v>0</v>
       </c>
       <c r="Z40" t="s">
@@ -3044,13 +3158,37 @@
         <v>22</v>
       </c>
       <c r="AE40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF40" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM40" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f>O41</f>
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -3070,15 +3208,15 @@
       </c>
       <c r="G41" s="11">
         <f>E41*(A41-1) + D41 -2*B41</f>
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="H41" s="19"/>
       <c r="I41" s="1">
         <f>W41</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="J41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41">
         <v>1</v>
@@ -3087,20 +3225,20 @@
         <v>4</v>
       </c>
       <c r="M41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N41">
         <f>O41/I41</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O41" s="2">
         <f>M41*(I41-1) + L41 -2*J41</f>
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="P41" s="19"/>
-      <c r="Q41" s="15">
+      <c r="Q41" s="1">
         <f>AE41</f>
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="R41">
         <v>1</v>
@@ -3109,43 +3247,68 @@
         <v>1</v>
       </c>
       <c r="T41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U41">
         <v>2</v>
       </c>
       <c r="V41">
         <f>W41/Q41</f>
-        <v>1.9393939393939394</v>
+        <v>2</v>
       </c>
       <c r="W41" s="2">
         <f>U41*(Q41-1) + T41 -2*R41</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="X41" s="19"/>
-      <c r="Y41" s="1">
-        <f>AE34</f>
-        <v>16</v>
-      </c>
-      <c r="Z41" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA41" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB41" s="4">
-        <v>3</v>
-      </c>
-      <c r="AC41" s="4">
+      <c r="Y41" s="15">
+        <f>AM41</f>
+        <v>8</v>
+      </c>
+      <c r="Z41">
+        <v>1</v>
+      </c>
+      <c r="AA41">
+        <v>1</v>
+      </c>
+      <c r="AB41">
+        <v>4</v>
+      </c>
+      <c r="AC41">
         <v>2</v>
       </c>
       <c r="AD41">
         <f>AE41/Y41</f>
-        <v>2.0625</v>
+        <v>2</v>
       </c>
       <c r="AE41" s="2">
         <f>AC41*(Y41-1) + AB41 -2*Z41</f>
-        <v>33</v>
+        <v>16</v>
+      </c>
+      <c r="AF41" s="19"/>
+      <c r="AG41" s="1">
+        <f>AM34</f>
+        <v>4</v>
+      </c>
+      <c r="AH41">
+        <v>0</v>
+      </c>
+      <c r="AI41">
+        <v>1</v>
+      </c>
+      <c r="AJ41">
+        <v>2</v>
+      </c>
+      <c r="AK41">
+        <v>2</v>
+      </c>
+      <c r="AL41">
+        <f>AM41/AG41</f>
+        <v>2</v>
+      </c>
+      <c r="AM41" s="2">
+        <f>AK41*(AG41-1) + AJ41 -2*AH41</f>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
@@ -3193,7 +3356,7 @@
         <v>7</v>
       </c>
       <c r="P42" s="19"/>
-      <c r="Q42" s="15" t="s">
+      <c r="Q42" s="1" t="s">
         <v>6</v>
       </c>
       <c r="R42" t="s">
@@ -3215,7 +3378,7 @@
         <v>7</v>
       </c>
       <c r="X42" s="19"/>
-      <c r="Y42" s="1" t="s">
+      <c r="Y42" s="15" t="s">
         <v>6</v>
       </c>
       <c r="Z42" t="s">
@@ -3234,13 +3397,35 @@
         <v>22</v>
       </c>
       <c r="AE42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF42" s="19"/>
+      <c r="AG42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM42" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <f>O43</f>
-        <v>320</v>
+        <v>80</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
@@ -3260,37 +3445,37 @@
       </c>
       <c r="G43" s="12">
         <f>E43*(A43-1) + D43 -2*B43</f>
-        <v>640</v>
+        <v>160</v>
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="3">
         <f>W43</f>
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="J43" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="4">
         <v>1</v>
       </c>
       <c r="L43" s="4">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="M43" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N43" s="4">
         <f>O43/I43</f>
-        <v>4.1025641025641022</v>
+        <v>2</v>
       </c>
       <c r="O43" s="5">
         <f>M43*(I43-1) + L43 -2*J43</f>
-        <v>320</v>
+        <v>80</v>
       </c>
       <c r="P43" s="19"/>
-      <c r="Q43" s="16">
+      <c r="Q43" s="3">
         <f>AE43</f>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="R43" s="4">
         <v>1</v>
@@ -3299,43 +3484,68 @@
         <v>1</v>
       </c>
       <c r="T43" s="4">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="U43" s="4">
         <v>2</v>
       </c>
       <c r="V43" s="4">
         <f>W43/Q43</f>
-        <v>2.3636363636363638</v>
+        <v>2</v>
       </c>
       <c r="W43" s="5">
         <f>U43*(Q43-1) + T43 -2*R43</f>
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="X43" s="19"/>
-      <c r="Y43" s="3">
-        <f>AE36</f>
-        <v>16</v>
+      <c r="Y43" s="16">
+        <f>AM43</f>
+        <v>10</v>
       </c>
       <c r="Z43" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA43" s="4">
         <v>1</v>
       </c>
       <c r="AB43" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC43" s="4">
         <v>2</v>
       </c>
       <c r="AD43" s="4">
         <f>AE43/Y43</f>
-        <v>2.0625</v>
+        <v>2</v>
       </c>
       <c r="AE43" s="5">
         <f>AC43*(Y43-1) + AB43 -2*Z43</f>
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="AF43" s="19"/>
+      <c r="AG43" s="3">
+        <f>AM36</f>
+        <v>5</v>
+      </c>
+      <c r="AH43" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ43" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK43" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL43" s="4">
+        <f>AM43/AG43</f>
+        <v>2</v>
+      </c>
+      <c r="AM43" s="5">
+        <f>AK43*(AG43-1) + AJ43 -2*AH43</f>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3350,59 +3560,47 @@
       <c r="B45" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="H45" s="8"/>
       <c r="P45" s="8"/>
       <c r="X45" s="8"/>
     </row>
     <row r="46" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="23"/>
-      <c r="I46" s="21" t="s">
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="22"/>
+      <c r="I46" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="23"/>
-      <c r="Q46" s="21" t="s">
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="22"/>
+      <c r="Q46" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R46" s="22"/>
-      <c r="S46" s="22"/>
-      <c r="T46" s="22"/>
-      <c r="U46" s="22"/>
-      <c r="V46" s="22"/>
-      <c r="W46" s="23"/>
-      <c r="Y46" s="21" t="s">
+      <c r="R46" s="21"/>
+      <c r="S46" s="21"/>
+      <c r="T46" s="21"/>
+      <c r="U46" s="21"/>
+      <c r="V46" s="21"/>
+      <c r="W46" s="22"/>
+      <c r="Y46" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Z46" s="22"/>
-      <c r="AA46" s="22"/>
-      <c r="AB46" s="22"/>
-      <c r="AC46" s="22"/>
-      <c r="AD46" s="22"/>
-      <c r="AE46" s="23"/>
-      <c r="AG46" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH46" s="22"/>
-      <c r="AI46" s="22"/>
-      <c r="AJ46" s="22"/>
-      <c r="AK46" s="22"/>
-      <c r="AL46" s="22"/>
-      <c r="AM46" s="23"/>
+      <c r="Z46" s="21"/>
+      <c r="AA46" s="21"/>
+      <c r="AB46" s="21"/>
+      <c r="AC46" s="21"/>
+      <c r="AD46" s="21"/>
+      <c r="AE46" s="22"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
@@ -3471,7 +3669,7 @@
       <c r="V47" t="s">
         <v>21</v>
       </c>
-      <c r="W47" s="2" t="s">
+      <c r="W47" s="13" t="s">
         <v>5</v>
       </c>
       <c r="X47" s="19" t="s">
@@ -3495,31 +3693,7 @@
       <c r="AD47" t="s">
         <v>21</v>
       </c>
-      <c r="AE47" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF47" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH47" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI47" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ47" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK47" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL47" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM47" s="2" t="s">
+      <c r="AE47" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3553,7 +3727,7 @@
         <v>256</v>
       </c>
       <c r="J48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48">
         <v>1</v>
@@ -3562,20 +3736,20 @@
         <v>4</v>
       </c>
       <c r="M48">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N48">
         <f>I48/O48</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O48" s="2">
         <f>((I48 + 2 * J48 - K48*(L48-1) -1) / M48 )+ 1</f>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="P48" s="19"/>
       <c r="Q48" s="1">
         <f>O48</f>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="R48">
         <v>1</v>
@@ -3584,67 +3758,42 @@
         <v>1</v>
       </c>
       <c r="T48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U48">
         <v>2</v>
       </c>
       <c r="V48">
         <f>Q48/W48</f>
-        <v>2</v>
-      </c>
-      <c r="W48" s="2">
-        <f>((Q48 + 2 * R48 - S48*(T48-1) -1) / U48 )+ 1</f>
-        <v>64</v>
+        <v>1.9393939393939394</v>
+      </c>
+      <c r="W48" s="13">
+        <f>(Q48 + 2 * R48 - S48*(T48-1) -1) / U48 + 1</f>
+        <v>33</v>
       </c>
       <c r="X48" s="19"/>
       <c r="Y48" s="1">
         <f>W48</f>
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="Z48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA48">
         <v>1</v>
       </c>
       <c r="AB48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC48">
         <v>2</v>
       </c>
       <c r="AD48">
         <f>Y48/AE48</f>
-        <v>2</v>
-      </c>
-      <c r="AE48" s="13">
+        <v>2.0625</v>
+      </c>
+      <c r="AE48" s="2">
         <f>(Y48 + 2 * Z48 - AA48*(AB48-1) -1) / AC48 + 1</f>
-        <v>32</v>
-      </c>
-      <c r="AF48" s="19"/>
-      <c r="AG48" s="1">
-        <f>AE48</f>
-        <v>32</v>
-      </c>
-      <c r="AH48">
-        <v>0</v>
-      </c>
-      <c r="AI48">
-        <v>1</v>
-      </c>
-      <c r="AJ48">
-        <v>2</v>
-      </c>
-      <c r="AK48">
-        <v>2</v>
-      </c>
-      <c r="AL48">
-        <f>AG48/AM48</f>
-        <v>2</v>
-      </c>
-      <c r="AM48" s="2">
-        <f>(AG48 + 2 * AH48 - AI48*(AJ48-1) -1) / AK48 + 1</f>
         <v>16</v>
       </c>
     </row>
@@ -3711,7 +3860,7 @@
       <c r="V49" t="s">
         <v>21</v>
       </c>
-      <c r="W49" s="2" t="s">
+      <c r="W49" s="13" t="s">
         <v>7</v>
       </c>
       <c r="X49" s="19"/>
@@ -3733,29 +3882,7 @@
       <c r="AD49" t="s">
         <v>21</v>
       </c>
-      <c r="AE49" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF49" s="19"/>
-      <c r="AG49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH49" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ49" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK49" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL49" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM49" s="2" t="s">
+      <c r="AE49" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3789,29 +3916,29 @@
         <v>320</v>
       </c>
       <c r="J50" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K50" s="4">
         <v>1</v>
       </c>
       <c r="L50" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="M50" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N50" s="4">
         <f>I50/O50</f>
-        <v>2</v>
+        <v>4.1025641025641022</v>
       </c>
       <c r="O50" s="5">
         <f>(I50 + 2 * J50 - K50*(L50-1) -1) / M50 + 1</f>
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="P50" s="19"/>
       <c r="Q50" s="3">
         <f>O50</f>
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="R50" s="4">
         <v>1</v>
@@ -3820,138 +3947,104 @@
         <v>1</v>
       </c>
       <c r="T50" s="4">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="U50" s="4">
         <v>2</v>
       </c>
       <c r="V50" s="4">
         <f>Q50/W50</f>
-        <v>2</v>
-      </c>
-      <c r="W50" s="5">
+        <v>2.3636363636363638</v>
+      </c>
+      <c r="W50" s="14">
         <f>(Q50 + 2 * R50 - S50*(T50-1) -1) / U50 + 1</f>
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="X50" s="19"/>
       <c r="Y50" s="3">
         <f>W50</f>
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="Z50" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA50" s="4">
         <v>1</v>
       </c>
       <c r="AB50" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC50" s="4">
         <v>2</v>
       </c>
       <c r="AD50" s="4">
         <f>Y50/AE50</f>
-        <v>2</v>
-      </c>
-      <c r="AE50" s="14">
+        <v>2.0625</v>
+      </c>
+      <c r="AE50" s="5">
         <f>(Y50 + 2 * Z50 - AA50*(AB50-1) -1) / AC50 + 1</f>
-        <v>40</v>
-      </c>
-      <c r="AF50" s="19"/>
-      <c r="AG50" s="3">
-        <f>AE50</f>
-        <v>40</v>
-      </c>
-      <c r="AH50" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI50" s="4">
-        <v>1</v>
-      </c>
-      <c r="AJ50" s="4">
-        <v>2</v>
-      </c>
-      <c r="AK50" s="4">
-        <v>2</v>
-      </c>
-      <c r="AL50" s="4">
-        <f>AG50/AM50</f>
-        <v>2</v>
-      </c>
-      <c r="AM50" s="5">
-        <f>(AG50 + 2 * AH50 - AI50*(AJ50-1) -1) / AK50 + 1</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AG51" s="24" t="s">
+      <c r="Y51" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="AH51" s="24"/>
-      <c r="AI51" s="24"/>
-      <c r="AJ51" s="24"/>
-      <c r="AK51" s="24"/>
-      <c r="AL51" s="24"/>
-      <c r="AM51" s="24"/>
+      <c r="Z51" s="23"/>
+      <c r="AA51" s="23"/>
+      <c r="AB51" s="23"/>
+      <c r="AC51" s="23"/>
+      <c r="AD51" s="23"/>
+      <c r="AE51" s="23"/>
     </row>
     <row r="52" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG52" s="20" t="s">
+      <c r="Y52" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AH52" s="20"/>
-      <c r="AI52" s="20"/>
-      <c r="AJ52" s="20"/>
-      <c r="AK52" s="20"/>
-      <c r="AL52" s="20"/>
-      <c r="AM52" s="20"/>
+      <c r="Z52" s="24"/>
+      <c r="AA52" s="24"/>
+      <c r="AB52" s="24"/>
+      <c r="AC52" s="24"/>
+      <c r="AD52" s="24"/>
+      <c r="AE52" s="24"/>
     </row>
     <row r="53" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="23"/>
-      <c r="I53" s="21" t="s">
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="22"/>
+      <c r="I53" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="22"/>
-      <c r="O53" s="23"/>
-      <c r="Q53" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="R53" s="22"/>
-      <c r="S53" s="22"/>
-      <c r="T53" s="22"/>
-      <c r="U53" s="22"/>
-      <c r="V53" s="22"/>
-      <c r="W53" s="23"/>
-      <c r="Y53" s="21" t="s">
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="21"/>
+      <c r="O53" s="22"/>
+      <c r="Q53" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="R53" s="21"/>
+      <c r="S53" s="21"/>
+      <c r="T53" s="21"/>
+      <c r="U53" s="21"/>
+      <c r="V53" s="21"/>
+      <c r="W53" s="22"/>
+      <c r="Y53" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="Z53" s="22"/>
-      <c r="AA53" s="22"/>
-      <c r="AB53" s="22"/>
-      <c r="AC53" s="22"/>
-      <c r="AD53" s="22"/>
-      <c r="AE53" s="23"/>
-      <c r="AG53" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH53" s="22"/>
-      <c r="AI53" s="22"/>
-      <c r="AJ53" s="22"/>
-      <c r="AK53" s="22"/>
-      <c r="AL53" s="22"/>
-      <c r="AM53" s="23"/>
+      <c r="Z53" s="21"/>
+      <c r="AA53" s="21"/>
+      <c r="AB53" s="21"/>
+      <c r="AC53" s="21"/>
+      <c r="AD53" s="21"/>
+      <c r="AE53" s="22"/>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
@@ -4002,7 +4095,7 @@
       <c r="P54" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="Q54" s="1" t="s">
+      <c r="Q54" s="15" t="s">
         <v>0</v>
       </c>
       <c r="R54" t="s">
@@ -4026,7 +4119,7 @@
       <c r="X54" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="Y54" s="15" t="s">
+      <c r="Y54" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Z54" t="s">
@@ -4045,30 +4138,6 @@
         <v>22</v>
       </c>
       <c r="AE54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF54" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH54" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI54" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ54" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK54" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL54" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM54" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4100,10 +4169,10 @@
       <c r="H55" s="19"/>
       <c r="I55" s="1">
         <f>W55</f>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -4112,20 +4181,20 @@
         <v>4</v>
       </c>
       <c r="M55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N55">
         <f>O55/I55</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O55" s="2">
         <f>M55*(I55-1) + L55 -2*J55</f>
         <v>256</v>
       </c>
       <c r="P55" s="19"/>
-      <c r="Q55" s="1">
+      <c r="Q55" s="15">
         <f>AE55</f>
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="R55">
         <v>1</v>
@@ -4134,68 +4203,43 @@
         <v>1</v>
       </c>
       <c r="T55">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U55">
         <v>2</v>
       </c>
       <c r="V55">
         <f>W55/Q55</f>
-        <v>2</v>
+        <v>1.9393939393939394</v>
       </c>
       <c r="W55" s="2">
         <f>U55*(Q55-1) + T55 -2*R55</f>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="X55" s="19"/>
-      <c r="Y55" s="15">
-        <f>AM55</f>
-        <v>32</v>
-      </c>
-      <c r="Z55">
-        <v>1</v>
-      </c>
-      <c r="AA55">
-        <v>1</v>
-      </c>
-      <c r="AB55">
-        <v>4</v>
-      </c>
-      <c r="AC55">
+      <c r="Y55" s="1">
+        <f>AE48</f>
+        <v>16</v>
+      </c>
+      <c r="Z55" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB55" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC55" s="4">
         <v>2</v>
       </c>
       <c r="AD55">
         <f>AE55/Y55</f>
-        <v>2</v>
+        <v>2.0625</v>
       </c>
       <c r="AE55" s="2">
         <f>AC55*(Y55-1) + AB55 -2*Z55</f>
-        <v>64</v>
-      </c>
-      <c r="AF55" s="19"/>
-      <c r="AG55" s="1">
-        <f>AM48</f>
-        <v>16</v>
-      </c>
-      <c r="AH55">
-        <v>0</v>
-      </c>
-      <c r="AI55">
-        <v>1</v>
-      </c>
-      <c r="AJ55">
-        <v>2</v>
-      </c>
-      <c r="AK55">
-        <v>2</v>
-      </c>
-      <c r="AL55">
-        <f>AM55/AG55</f>
-        <v>2</v>
-      </c>
-      <c r="AM55" s="2">
-        <f>AK55*(AG55-1) + AJ55 -2*AH55</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.25">
@@ -4243,7 +4287,7 @@
         <v>7</v>
       </c>
       <c r="P56" s="19"/>
-      <c r="Q56" s="1" t="s">
+      <c r="Q56" s="15" t="s">
         <v>6</v>
       </c>
       <c r="R56" t="s">
@@ -4265,7 +4309,7 @@
         <v>7</v>
       </c>
       <c r="X56" s="19"/>
-      <c r="Y56" s="15" t="s">
+      <c r="Y56" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Z56" t="s">
@@ -4284,28 +4328,6 @@
         <v>22</v>
       </c>
       <c r="AE56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF56" s="19"/>
-      <c r="AG56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH56" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI56" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ56" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK56" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL56" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM56" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4337,32 +4359,32 @@
       <c r="H57" s="19"/>
       <c r="I57" s="3">
         <f>W57</f>
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="J57" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57" s="4">
         <v>1</v>
       </c>
       <c r="L57" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="M57" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N57" s="4">
         <f>O57/I57</f>
-        <v>2</v>
+        <v>4.1025641025641022</v>
       </c>
       <c r="O57" s="5">
         <f>M57*(I57-1) + L57 -2*J57</f>
         <v>320</v>
       </c>
       <c r="P57" s="19"/>
-      <c r="Q57" s="3">
+      <c r="Q57" s="16">
         <f>AE57</f>
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="R57" s="4">
         <v>1</v>
@@ -4371,108 +4393,1180 @@
         <v>1</v>
       </c>
       <c r="T57" s="4">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="U57" s="4">
         <v>2</v>
       </c>
       <c r="V57" s="4">
         <f>W57/Q57</f>
-        <v>2</v>
+        <v>2.3636363636363638</v>
       </c>
       <c r="W57" s="5">
         <f>U57*(Q57-1) + T57 -2*R57</f>
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="X57" s="19"/>
-      <c r="Y57" s="16">
-        <f>AM57</f>
-        <v>40</v>
+      <c r="Y57" s="3">
+        <f>AE50</f>
+        <v>16</v>
       </c>
       <c r="Z57" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA57" s="4">
         <v>1</v>
       </c>
       <c r="AB57" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC57" s="4">
         <v>2</v>
       </c>
       <c r="AD57" s="4">
         <f>AE57/Y57</f>
-        <v>2</v>
+        <v>2.0625</v>
       </c>
       <c r="AE57" s="5">
         <f>AC57*(Y57-1) + AB57 -2*Z57</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="X58" s="8"/>
+    </row>
+    <row r="59" spans="1:39" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="X59" s="8"/>
+    </row>
+    <row r="60" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="22"/>
+      <c r="I60" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
+      <c r="M60" s="21"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="22"/>
+      <c r="Q60" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R60" s="21"/>
+      <c r="S60" s="21"/>
+      <c r="T60" s="21"/>
+      <c r="U60" s="21"/>
+      <c r="V60" s="21"/>
+      <c r="W60" s="22"/>
+      <c r="Y60" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z60" s="21"/>
+      <c r="AA60" s="21"/>
+      <c r="AB60" s="21"/>
+      <c r="AC60" s="21"/>
+      <c r="AD60" s="21"/>
+      <c r="AE60" s="22"/>
+      <c r="AG60" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH60" s="21"/>
+      <c r="AI60" s="21"/>
+      <c r="AJ60" s="21"/>
+      <c r="AK60" s="21"/>
+      <c r="AL60" s="21"/>
+      <c r="AM60" s="22"/>
+    </row>
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" t="s">
+        <v>21</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H61" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J61" t="s">
+        <v>1</v>
+      </c>
+      <c r="K61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L61" t="s">
+        <v>3</v>
+      </c>
+      <c r="M61" t="s">
+        <v>4</v>
+      </c>
+      <c r="N61" t="s">
+        <v>21</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P61" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R61" t="s">
+        <v>1</v>
+      </c>
+      <c r="S61" t="s">
+        <v>2</v>
+      </c>
+      <c r="T61" t="s">
+        <v>3</v>
+      </c>
+      <c r="U61" t="s">
+        <v>4</v>
+      </c>
+      <c r="V61" t="s">
+        <v>21</v>
+      </c>
+      <c r="W61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X61" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE61" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF61" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH61" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI61" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ61" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK61" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL61" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM61" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>512</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <f>A62/G62</f>
+        <v>2</v>
+      </c>
+      <c r="G62" s="2">
+        <f>(A62 + 2 * B62 - C62*(D62-1) -1) / E62 + 1</f>
+        <v>256</v>
+      </c>
+      <c r="H62" s="19"/>
+      <c r="I62" s="1">
+        <f>G62</f>
+        <v>256</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>4</v>
+      </c>
+      <c r="M62">
+        <v>2</v>
+      </c>
+      <c r="N62">
+        <f>I62/O62</f>
+        <v>2</v>
+      </c>
+      <c r="O62" s="2">
+        <f>((I62 + 2 * J62 - K62*(L62-1) -1) / M62 )+ 1</f>
+        <v>128</v>
+      </c>
+      <c r="P62" s="19"/>
+      <c r="Q62" s="1">
+        <f>O62</f>
+        <v>128</v>
+      </c>
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <v>1</v>
+      </c>
+      <c r="T62">
+        <v>4</v>
+      </c>
+      <c r="U62">
+        <v>2</v>
+      </c>
+      <c r="V62">
+        <f>Q62/W62</f>
+        <v>2</v>
+      </c>
+      <c r="W62" s="2">
+        <f>((Q62 + 2 * R62 - S62*(T62-1) -1) / U62 )+ 1</f>
+        <v>64</v>
+      </c>
+      <c r="X62" s="19"/>
+      <c r="Y62" s="1">
+        <f>W62</f>
+        <v>64</v>
+      </c>
+      <c r="Z62">
+        <v>1</v>
+      </c>
+      <c r="AA62">
+        <v>1</v>
+      </c>
+      <c r="AB62">
+        <v>4</v>
+      </c>
+      <c r="AC62">
+        <v>2</v>
+      </c>
+      <c r="AD62">
+        <f>Y62/AE62</f>
+        <v>2</v>
+      </c>
+      <c r="AE62" s="13">
+        <f>(Y62 + 2 * Z62 - AA62*(AB62-1) -1) / AC62 + 1</f>
+        <v>32</v>
+      </c>
+      <c r="AF62" s="19"/>
+      <c r="AG62" s="1">
+        <f>AE62</f>
+        <v>32</v>
+      </c>
+      <c r="AH62">
+        <v>0</v>
+      </c>
+      <c r="AI62">
+        <v>1</v>
+      </c>
+      <c r="AJ62">
+        <v>2</v>
+      </c>
+      <c r="AK62">
+        <v>2</v>
+      </c>
+      <c r="AL62">
+        <f>AG62/AM62</f>
+        <v>2</v>
+      </c>
+      <c r="AM62" s="2">
+        <f>(AG62 + 2 * AH62 - AI62*(AJ62-1) -1) / AK62 + 1</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" t="s">
+        <v>21</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="19"/>
+      <c r="I63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J63" t="s">
+        <v>1</v>
+      </c>
+      <c r="K63" t="s">
+        <v>2</v>
+      </c>
+      <c r="L63" t="s">
+        <v>3</v>
+      </c>
+      <c r="M63" t="s">
+        <v>4</v>
+      </c>
+      <c r="N63" t="s">
+        <v>21</v>
+      </c>
+      <c r="O63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P63" s="19"/>
+      <c r="Q63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R63" t="s">
+        <v>1</v>
+      </c>
+      <c r="S63" t="s">
+        <v>2</v>
+      </c>
+      <c r="T63" t="s">
+        <v>3</v>
+      </c>
+      <c r="U63" t="s">
+        <v>4</v>
+      </c>
+      <c r="V63" t="s">
+        <v>21</v>
+      </c>
+      <c r="W63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X63" s="19"/>
+      <c r="Y63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC63" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE63" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF63" s="19"/>
+      <c r="AG63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH63" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI63" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ63" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK63" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL63" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM63" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A64" s="10">
+        <v>640</v>
+      </c>
+      <c r="B64" s="4">
+        <v>1</v>
+      </c>
+      <c r="C64" s="4">
+        <v>1</v>
+      </c>
+      <c r="D64" s="4">
+        <v>4</v>
+      </c>
+      <c r="E64" s="4">
+        <v>2</v>
+      </c>
+      <c r="F64" s="4">
+        <f>A64/G64</f>
+        <v>2</v>
+      </c>
+      <c r="G64" s="5">
+        <f>(A64 + 2 * B64 - C64*(D64-1) -1) / E64 + 1</f>
+        <v>320</v>
+      </c>
+      <c r="H64" s="19"/>
+      <c r="I64" s="3">
+        <f>G64</f>
+        <v>320</v>
+      </c>
+      <c r="J64" s="4">
+        <v>1</v>
+      </c>
+      <c r="K64" s="4">
+        <v>1</v>
+      </c>
+      <c r="L64" s="4">
+        <v>4</v>
+      </c>
+      <c r="M64" s="4">
+        <v>2</v>
+      </c>
+      <c r="N64" s="4">
+        <f>I64/O64</f>
+        <v>2</v>
+      </c>
+      <c r="O64" s="5">
+        <f>(I64 + 2 * J64 - K64*(L64-1) -1) / M64 + 1</f>
+        <v>160</v>
+      </c>
+      <c r="P64" s="19"/>
+      <c r="Q64" s="3">
+        <f>O64</f>
+        <v>160</v>
+      </c>
+      <c r="R64" s="4">
+        <v>1</v>
+      </c>
+      <c r="S64" s="4">
+        <v>1</v>
+      </c>
+      <c r="T64" s="4">
+        <v>4</v>
+      </c>
+      <c r="U64" s="4">
+        <v>2</v>
+      </c>
+      <c r="V64" s="4">
+        <f>Q64/W64</f>
+        <v>2</v>
+      </c>
+      <c r="W64" s="5">
+        <f>(Q64 + 2 * R64 - S64*(T64-1) -1) / U64 + 1</f>
         <v>80</v>
       </c>
-      <c r="AF57" s="19"/>
-      <c r="AG57" s="3">
-        <f>AM50</f>
+      <c r="X64" s="19"/>
+      <c r="Y64" s="3">
+        <f>W64</f>
+        <v>80</v>
+      </c>
+      <c r="Z64" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA64" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB64" s="4">
+        <v>4</v>
+      </c>
+      <c r="AC64" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD64" s="4">
+        <f>Y64/AE64</f>
+        <v>2</v>
+      </c>
+      <c r="AE64" s="14">
+        <f>(Y64 + 2 * Z64 - AA64*(AB64-1) -1) / AC64 + 1</f>
+        <v>40</v>
+      </c>
+      <c r="AF64" s="19"/>
+      <c r="AG64" s="3">
+        <f>AE64</f>
+        <v>40</v>
+      </c>
+      <c r="AH64" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI64" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ64" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK64" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL64" s="4">
+        <f>AG64/AM64</f>
+        <v>2</v>
+      </c>
+      <c r="AM64" s="5">
+        <f>(AG64 + 2 * AH64 - AI64*(AJ64-1) -1) / AK64 + 1</f>
         <v>20</v>
       </c>
-      <c r="AH57" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI57" s="4">
-        <v>1</v>
-      </c>
-      <c r="AJ57" s="4">
-        <v>2</v>
-      </c>
-      <c r="AK57" s="4">
-        <v>2</v>
-      </c>
-      <c r="AL57" s="4">
-        <f>AM57/AG57</f>
-        <v>2</v>
-      </c>
-      <c r="AM57" s="5">
-        <f>AK57*(AG57-1) + AJ57 -2*AH57</f>
+    </row>
+    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AG65" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH65" s="23"/>
+      <c r="AI65" s="23"/>
+      <c r="AJ65" s="23"/>
+      <c r="AK65" s="23"/>
+      <c r="AL65" s="23"/>
+      <c r="AM65" s="23"/>
+    </row>
+    <row r="66" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG66" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH66" s="24"/>
+      <c r="AI66" s="24"/>
+      <c r="AJ66" s="24"/>
+      <c r="AK66" s="24"/>
+      <c r="AL66" s="24"/>
+      <c r="AM66" s="24"/>
+    </row>
+    <row r="67" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="22"/>
+      <c r="I67" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="21"/>
+      <c r="N67" s="21"/>
+      <c r="O67" s="22"/>
+      <c r="Q67" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R67" s="21"/>
+      <c r="S67" s="21"/>
+      <c r="T67" s="21"/>
+      <c r="U67" s="21"/>
+      <c r="V67" s="21"/>
+      <c r="W67" s="22"/>
+      <c r="Y67" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z67" s="21"/>
+      <c r="AA67" s="21"/>
+      <c r="AB67" s="21"/>
+      <c r="AC67" s="21"/>
+      <c r="AD67" s="21"/>
+      <c r="AE67" s="22"/>
+      <c r="AG67" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH67" s="21"/>
+      <c r="AI67" s="21"/>
+      <c r="AJ67" s="21"/>
+      <c r="AK67" s="21"/>
+      <c r="AL67" s="21"/>
+      <c r="AM67" s="22"/>
+    </row>
+    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>1</v>
+      </c>
+      <c r="K68" t="s">
+        <v>2</v>
+      </c>
+      <c r="L68" t="s">
+        <v>3</v>
+      </c>
+      <c r="M68" t="s">
+        <v>4</v>
+      </c>
+      <c r="N68" t="s">
+        <v>22</v>
+      </c>
+      <c r="O68" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P68" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R68" t="s">
+        <v>1</v>
+      </c>
+      <c r="S68" t="s">
+        <v>2</v>
+      </c>
+      <c r="T68" t="s">
+        <v>3</v>
+      </c>
+      <c r="U68" t="s">
+        <v>4</v>
+      </c>
+      <c r="V68" t="s">
+        <v>22</v>
+      </c>
+      <c r="W68" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X68" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y68" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD68" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE68" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF68" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH68" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI68" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ68" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK68" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL68" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM68" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <f>O69</f>
+        <v>256</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>4</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69">
+        <f>G69/A69</f>
+        <v>2</v>
+      </c>
+      <c r="G69" s="11">
+        <f>E69*(A69-1) + D69 -2*B69</f>
+        <v>512</v>
+      </c>
+      <c r="H69" s="19"/>
+      <c r="I69" s="1">
+        <f>W69</f>
+        <v>128</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>4</v>
+      </c>
+      <c r="M69">
+        <v>2</v>
+      </c>
+      <c r="N69">
+        <f>O69/I69</f>
+        <v>2</v>
+      </c>
+      <c r="O69" s="2">
+        <f>M69*(I69-1) + L69 -2*J69</f>
+        <v>256</v>
+      </c>
+      <c r="P69" s="19"/>
+      <c r="Q69" s="1">
+        <f>AE69</f>
+        <v>64</v>
+      </c>
+      <c r="R69">
+        <v>1</v>
+      </c>
+      <c r="S69">
+        <v>1</v>
+      </c>
+      <c r="T69">
+        <v>4</v>
+      </c>
+      <c r="U69">
+        <v>2</v>
+      </c>
+      <c r="V69">
+        <f>W69/Q69</f>
+        <v>2</v>
+      </c>
+      <c r="W69" s="2">
+        <f>U69*(Q69-1) + T69 -2*R69</f>
+        <v>128</v>
+      </c>
+      <c r="X69" s="19"/>
+      <c r="Y69" s="15">
+        <f>AM69</f>
+        <v>32</v>
+      </c>
+      <c r="Z69">
+        <v>1</v>
+      </c>
+      <c r="AA69">
+        <v>1</v>
+      </c>
+      <c r="AB69">
+        <v>4</v>
+      </c>
+      <c r="AC69">
+        <v>2</v>
+      </c>
+      <c r="AD69">
+        <f>AE69/Y69</f>
+        <v>2</v>
+      </c>
+      <c r="AE69" s="2">
+        <f>AC69*(Y69-1) + AB69 -2*Z69</f>
+        <v>64</v>
+      </c>
+      <c r="AF69" s="19"/>
+      <c r="AG69" s="1">
+        <f>AM62</f>
+        <v>16</v>
+      </c>
+      <c r="AH69">
+        <v>0</v>
+      </c>
+      <c r="AI69">
+        <v>1</v>
+      </c>
+      <c r="AJ69">
+        <v>2</v>
+      </c>
+      <c r="AK69">
+        <v>2</v>
+      </c>
+      <c r="AL69">
+        <f>AM69/AG69</f>
+        <v>2</v>
+      </c>
+      <c r="AM69" s="2">
+        <f>AK69*(AG69-1) + AJ69 -2*AH69</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" t="s">
+        <v>22</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" s="19"/>
+      <c r="I70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J70" t="s">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>2</v>
+      </c>
+      <c r="L70" t="s">
+        <v>3</v>
+      </c>
+      <c r="M70" t="s">
+        <v>4</v>
+      </c>
+      <c r="N70" t="s">
+        <v>22</v>
+      </c>
+      <c r="O70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P70" s="19"/>
+      <c r="Q70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R70" t="s">
+        <v>1</v>
+      </c>
+      <c r="S70" t="s">
+        <v>2</v>
+      </c>
+      <c r="T70" t="s">
+        <v>3</v>
+      </c>
+      <c r="U70" t="s">
+        <v>4</v>
+      </c>
+      <c r="V70" t="s">
+        <v>22</v>
+      </c>
+      <c r="W70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X70" s="19"/>
+      <c r="Y70" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA70" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF70" s="19"/>
+      <c r="AG70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH70" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI70" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ70" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK70" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL70" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM70" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <f>O71</f>
+        <v>320</v>
+      </c>
+      <c r="B71" s="4">
+        <v>1</v>
+      </c>
+      <c r="C71" s="4">
+        <v>1</v>
+      </c>
+      <c r="D71" s="4">
+        <v>4</v>
+      </c>
+      <c r="E71" s="4">
+        <v>2</v>
+      </c>
+      <c r="F71" s="4">
+        <f>G71/A71</f>
+        <v>2</v>
+      </c>
+      <c r="G71" s="12">
+        <f>E71*(A71-1) + D71 -2*B71</f>
+        <v>640</v>
+      </c>
+      <c r="H71" s="19"/>
+      <c r="I71" s="3">
+        <f>W71</f>
+        <v>160</v>
+      </c>
+      <c r="J71" s="4">
+        <v>1</v>
+      </c>
+      <c r="K71" s="4">
+        <v>1</v>
+      </c>
+      <c r="L71" s="4">
+        <v>4</v>
+      </c>
+      <c r="M71" s="4">
+        <v>2</v>
+      </c>
+      <c r="N71" s="4">
+        <f>O71/I71</f>
+        <v>2</v>
+      </c>
+      <c r="O71" s="5">
+        <f>M71*(I71-1) + L71 -2*J71</f>
+        <v>320</v>
+      </c>
+      <c r="P71" s="19"/>
+      <c r="Q71" s="3">
+        <f>AE71</f>
+        <v>80</v>
+      </c>
+      <c r="R71" s="4">
+        <v>1</v>
+      </c>
+      <c r="S71" s="4">
+        <v>1</v>
+      </c>
+      <c r="T71" s="4">
+        <v>4</v>
+      </c>
+      <c r="U71" s="4">
+        <v>2</v>
+      </c>
+      <c r="V71" s="4">
+        <f>W71/Q71</f>
+        <v>2</v>
+      </c>
+      <c r="W71" s="5">
+        <f>U71*(Q71-1) + T71 -2*R71</f>
+        <v>160</v>
+      </c>
+      <c r="X71" s="19"/>
+      <c r="Y71" s="16">
+        <f>AM71</f>
         <v>40</v>
       </c>
+      <c r="Z71" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA71" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB71" s="4">
+        <v>4</v>
+      </c>
+      <c r="AC71" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD71" s="4">
+        <f>AE71/Y71</f>
+        <v>2</v>
+      </c>
+      <c r="AE71" s="5">
+        <f>AC71*(Y71-1) + AB71 -2*Z71</f>
+        <v>80</v>
+      </c>
+      <c r="AF71" s="19"/>
+      <c r="AG71" s="3">
+        <f>AM64</f>
+        <v>20</v>
+      </c>
+      <c r="AH71" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI71" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ71" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK71" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL71" s="4">
+        <f>AM71/AG71</f>
+        <v>2</v>
+      </c>
+      <c r="AM71" s="5">
+        <f>AK71*(AG71-1) + AJ71 -2*AH71</f>
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="X54:X57"/>
-    <mergeCell ref="AF54:AF57"/>
-    <mergeCell ref="I46:O46"/>
-    <mergeCell ref="P47:P50"/>
-    <mergeCell ref="I53:O53"/>
-    <mergeCell ref="P54:P57"/>
-    <mergeCell ref="AG51:AM51"/>
-    <mergeCell ref="AG52:AM52"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="Q53:W53"/>
-    <mergeCell ref="Y53:AE53"/>
-    <mergeCell ref="AG53:AM53"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="Q46:W46"/>
-    <mergeCell ref="Y46:AE46"/>
-    <mergeCell ref="AG46:AM46"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="X47:X50"/>
-    <mergeCell ref="AF47:AF50"/>
+  <mergeCells count="88">
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="P40:P43"/>
+    <mergeCell ref="X40:X43"/>
+    <mergeCell ref="AG32:AM32"/>
+    <mergeCell ref="AF33:AF36"/>
+    <mergeCell ref="AG37:AM37"/>
+    <mergeCell ref="AG38:AM38"/>
+    <mergeCell ref="AG39:AM39"/>
+    <mergeCell ref="AF40:AF43"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="I39:O39"/>
+    <mergeCell ref="Q39:W39"/>
+    <mergeCell ref="Y39:AE39"/>
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="I32:O32"/>
     <mergeCell ref="Q32:W32"/>
     <mergeCell ref="Y32:AE32"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="I39:O39"/>
-    <mergeCell ref="Q39:W39"/>
-    <mergeCell ref="Y39:AE39"/>
     <mergeCell ref="H33:H36"/>
-    <mergeCell ref="H40:H43"/>
     <mergeCell ref="P33:P36"/>
     <mergeCell ref="X33:X36"/>
-    <mergeCell ref="Y37:AE37"/>
-    <mergeCell ref="Y38:AE38"/>
-    <mergeCell ref="X40:X43"/>
-    <mergeCell ref="P40:P43"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="P26:P29"/>
+    <mergeCell ref="X26:X29"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="P19:P22"/>
+    <mergeCell ref="X19:X22"/>
+    <mergeCell ref="Y24:AE24"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="I25:O25"/>
+    <mergeCell ref="Q25:W25"/>
+    <mergeCell ref="Y25:AE25"/>
+    <mergeCell ref="Y11:AE11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="P12:P15"/>
+    <mergeCell ref="X12:X15"/>
+    <mergeCell ref="Y23:AE23"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="I18:O18"/>
     <mergeCell ref="Q18:W18"/>
@@ -4489,22 +5583,42 @@
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="I11:O11"/>
     <mergeCell ref="Q11:W11"/>
-    <mergeCell ref="Y11:AE11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="P12:P15"/>
-    <mergeCell ref="X12:X15"/>
-    <mergeCell ref="Y23:AE23"/>
-    <mergeCell ref="Y24:AE24"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="I25:O25"/>
-    <mergeCell ref="Q25:W25"/>
-    <mergeCell ref="Y25:AE25"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="P26:P29"/>
-    <mergeCell ref="X26:X29"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="P19:P22"/>
-    <mergeCell ref="X19:X22"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="P47:P50"/>
+    <mergeCell ref="X47:X50"/>
+    <mergeCell ref="Y51:AE51"/>
+    <mergeCell ref="Y52:AE52"/>
+    <mergeCell ref="X54:X57"/>
+    <mergeCell ref="P54:P57"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="I46:O46"/>
+    <mergeCell ref="Q46:W46"/>
+    <mergeCell ref="Y46:AE46"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="I53:O53"/>
+    <mergeCell ref="Q53:W53"/>
+    <mergeCell ref="Y53:AE53"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="Q60:W60"/>
+    <mergeCell ref="Y60:AE60"/>
+    <mergeCell ref="AG60:AM60"/>
+    <mergeCell ref="H61:H64"/>
+    <mergeCell ref="X61:X64"/>
+    <mergeCell ref="AF61:AF64"/>
+    <mergeCell ref="AG65:AM65"/>
+    <mergeCell ref="AG66:AM66"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="Q67:W67"/>
+    <mergeCell ref="Y67:AE67"/>
+    <mergeCell ref="AG67:AM67"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="X68:X71"/>
+    <mergeCell ref="AF68:AF71"/>
+    <mergeCell ref="I60:O60"/>
+    <mergeCell ref="P61:P64"/>
+    <mergeCell ref="I67:O67"/>
+    <mergeCell ref="P68:P71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Jippiejayee, het werkt allemaal nog steeds niet, zelfs met MNIST niet
Cleaned a lot of stuff in the porcess
</commit_message>
<xml_diff>
--- a/Convolutional network size calculator.xlsx
+++ b/Convolutional network size calculator.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timva\Documents\GitHub\Sparse-recovery-of-IR-images-using-a-score-based-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A800E130-AD9A-457B-BD15-E21344A9CBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9270EEE8-3857-40DE-A707-75E4FE0AA1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B2DC737-34CF-420A-AF9A-B9F1BF30D588}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2B2DC737-34CF-420A-AF9A-B9F1BF30D588}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NCSN" sheetId="1" r:id="rId1"/>
+    <sheet name="MNIST" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="30">
   <si>
     <t>Hin</t>
   </si>
@@ -123,6 +124,9 @@
   </si>
   <si>
     <t>tConv 5</t>
+  </si>
+  <si>
+    <t>28x28</t>
   </si>
 </sst>
 </file>
@@ -673,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E69EC-ECC9-4653-A3EC-CA67F7716823}">
   <dimension ref="A1:AM71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W26" zoomScale="106" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40:P43"/>
+    <sheetView topLeftCell="A21" zoomScale="43" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AM71" sqref="A58:AM71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5531,42 +5535,42 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="P40:P43"/>
-    <mergeCell ref="X40:X43"/>
-    <mergeCell ref="AG32:AM32"/>
-    <mergeCell ref="AF33:AF36"/>
-    <mergeCell ref="AG37:AM37"/>
-    <mergeCell ref="AG38:AM38"/>
-    <mergeCell ref="AG39:AM39"/>
-    <mergeCell ref="AF40:AF43"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="I39:O39"/>
-    <mergeCell ref="Q39:W39"/>
-    <mergeCell ref="Y39:AE39"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="I32:O32"/>
-    <mergeCell ref="Q32:W32"/>
-    <mergeCell ref="Y32:AE32"/>
-    <mergeCell ref="H33:H36"/>
-    <mergeCell ref="P33:P36"/>
-    <mergeCell ref="X33:X36"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="P26:P29"/>
-    <mergeCell ref="X26:X29"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="P19:P22"/>
-    <mergeCell ref="X19:X22"/>
-    <mergeCell ref="Y24:AE24"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="I25:O25"/>
-    <mergeCell ref="Q25:W25"/>
-    <mergeCell ref="Y25:AE25"/>
-    <mergeCell ref="Y11:AE11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="P12:P15"/>
-    <mergeCell ref="X12:X15"/>
-    <mergeCell ref="Y23:AE23"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="X68:X71"/>
+    <mergeCell ref="AF68:AF71"/>
+    <mergeCell ref="I60:O60"/>
+    <mergeCell ref="P61:P64"/>
+    <mergeCell ref="I67:O67"/>
+    <mergeCell ref="P68:P71"/>
+    <mergeCell ref="AG65:AM65"/>
+    <mergeCell ref="AG66:AM66"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="Q67:W67"/>
+    <mergeCell ref="Y67:AE67"/>
+    <mergeCell ref="AG67:AM67"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="Q60:W60"/>
+    <mergeCell ref="Y60:AE60"/>
+    <mergeCell ref="AG60:AM60"/>
+    <mergeCell ref="H61:H64"/>
+    <mergeCell ref="X61:X64"/>
+    <mergeCell ref="AF61:AF64"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="I46:O46"/>
+    <mergeCell ref="Q46:W46"/>
+    <mergeCell ref="Y46:AE46"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="I53:O53"/>
+    <mergeCell ref="Q53:W53"/>
+    <mergeCell ref="Y53:AE53"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="P47:P50"/>
+    <mergeCell ref="X47:X50"/>
+    <mergeCell ref="Y51:AE51"/>
+    <mergeCell ref="Y52:AE52"/>
+    <mergeCell ref="X54:X57"/>
+    <mergeCell ref="P54:P57"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="I18:O18"/>
     <mergeCell ref="Q18:W18"/>
@@ -5583,42 +5587,1245 @@
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="I11:O11"/>
     <mergeCell ref="Q11:W11"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="P47:P50"/>
-    <mergeCell ref="X47:X50"/>
-    <mergeCell ref="Y51:AE51"/>
-    <mergeCell ref="Y52:AE52"/>
-    <mergeCell ref="X54:X57"/>
-    <mergeCell ref="P54:P57"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="I46:O46"/>
-    <mergeCell ref="Q46:W46"/>
-    <mergeCell ref="Y46:AE46"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="I53:O53"/>
-    <mergeCell ref="Q53:W53"/>
-    <mergeCell ref="Y53:AE53"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="Q60:W60"/>
-    <mergeCell ref="Y60:AE60"/>
-    <mergeCell ref="AG60:AM60"/>
-    <mergeCell ref="H61:H64"/>
-    <mergeCell ref="X61:X64"/>
-    <mergeCell ref="AF61:AF64"/>
-    <mergeCell ref="AG65:AM65"/>
-    <mergeCell ref="AG66:AM66"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="Q67:W67"/>
-    <mergeCell ref="Y67:AE67"/>
-    <mergeCell ref="AG67:AM67"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="X68:X71"/>
-    <mergeCell ref="AF68:AF71"/>
-    <mergeCell ref="I60:O60"/>
-    <mergeCell ref="P61:P64"/>
-    <mergeCell ref="I67:O67"/>
-    <mergeCell ref="P68:P71"/>
+    <mergeCell ref="Y11:AE11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="P12:P15"/>
+    <mergeCell ref="X12:X15"/>
+    <mergeCell ref="Y23:AE23"/>
+    <mergeCell ref="Y24:AE24"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="I25:O25"/>
+    <mergeCell ref="Q25:W25"/>
+    <mergeCell ref="Y25:AE25"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="P26:P29"/>
+    <mergeCell ref="X26:X29"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="P19:P22"/>
+    <mergeCell ref="X19:X22"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="I39:O39"/>
+    <mergeCell ref="Q39:W39"/>
+    <mergeCell ref="Y39:AE39"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="I32:O32"/>
+    <mergeCell ref="Q32:W32"/>
+    <mergeCell ref="Y32:AE32"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="P33:P36"/>
+    <mergeCell ref="X33:X36"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="P40:P43"/>
+    <mergeCell ref="X40:X43"/>
+    <mergeCell ref="AG32:AM32"/>
+    <mergeCell ref="AF33:AF36"/>
+    <mergeCell ref="AG37:AM37"/>
+    <mergeCell ref="AG38:AM38"/>
+    <mergeCell ref="AG39:AM39"/>
+    <mergeCell ref="AF40:AF43"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57EDBCC-9D54-4F0D-8FC8-82CD71FEE0A9}">
+  <dimension ref="A1:AM14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AI19" sqref="AI19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+    </row>
+    <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="7"/>
+    </row>
+    <row r="3" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="I3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="22"/>
+      <c r="Q3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="22"/>
+      <c r="Y3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="22"/>
+      <c r="AG3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="21"/>
+      <c r="AL3" s="21"/>
+      <c r="AM3" s="22"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f>A5/G5</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <f>(A5 + 2 * B5 - C5*(D5-1) -1) / E5 + 1</f>
+        <v>14</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="1">
+        <f>G5</f>
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <f>I5/O5</f>
+        <v>2</v>
+      </c>
+      <c r="O5" s="2">
+        <f>((I5 + 2 * J5 - K5*(L5-1) -1) / M5 )+ 1</f>
+        <v>7</v>
+      </c>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="1">
+        <f>O5</f>
+        <v>7</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <f>Q5/W5</f>
+        <v>1.75</v>
+      </c>
+      <c r="W5" s="2">
+        <f>((Q5 + 2 * R5 - S5*(T5-1) -1) / U5 )+ 1</f>
+        <v>4</v>
+      </c>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="1">
+        <f>W5</f>
+        <v>4</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>4</v>
+      </c>
+      <c r="AC5">
+        <v>2</v>
+      </c>
+      <c r="AD5">
+        <f>Y5/AE5</f>
+        <v>2</v>
+      </c>
+      <c r="AE5" s="13">
+        <f>(Y5 + 2 * Z5 - AA5*(AB5-1) -1) / AC5 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="1">
+        <f>AE5</f>
+        <v>2</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>2</v>
+      </c>
+      <c r="AK5">
+        <v>2</v>
+      </c>
+      <c r="AL5">
+        <f>AG5/AM5</f>
+        <v>2</v>
+      </c>
+      <c r="AM5" s="2">
+        <f>(AG5 + 2 * AH5 - AI5*(AJ5-1) -1) / AK5 + 1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V6" t="s">
+        <v>21</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>28</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <f>A7/G7</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="5">
+        <f>(A7 + 2 * B7 - C7*(D7-1) -1) / E7 + 1</f>
+        <v>14</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="3">
+        <f>G7</f>
+        <v>14</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>4</v>
+      </c>
+      <c r="M7" s="4">
+        <v>2</v>
+      </c>
+      <c r="N7" s="4">
+        <f>I7/O7</f>
+        <v>2</v>
+      </c>
+      <c r="O7" s="5">
+        <f>(I7 + 2 * J7 - K7*(L7-1) -1) / M7 + 1</f>
+        <v>7</v>
+      </c>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="3">
+        <f>O7</f>
+        <v>7</v>
+      </c>
+      <c r="R7" s="4">
+        <v>1</v>
+      </c>
+      <c r="S7" s="4">
+        <v>1</v>
+      </c>
+      <c r="T7" s="4">
+        <v>3</v>
+      </c>
+      <c r="U7" s="4">
+        <v>2</v>
+      </c>
+      <c r="V7" s="4">
+        <f>Q7/W7</f>
+        <v>1.75</v>
+      </c>
+      <c r="W7" s="5">
+        <f>(Q7 + 2 * R7 - S7*(T7-1) -1) / U7 + 1</f>
+        <v>4</v>
+      </c>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="3">
+        <f>W7</f>
+        <v>4</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="4">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="4">
+        <f>Y7/AE7</f>
+        <v>2</v>
+      </c>
+      <c r="AE7" s="14">
+        <f>(Y7 + 2 * Z7 - AA7*(AB7-1) -1) / AC7 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="3">
+        <f>AE7</f>
+        <v>2</v>
+      </c>
+      <c r="AH7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK7" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL7" s="4">
+        <f>AG7/AM7</f>
+        <v>2</v>
+      </c>
+      <c r="AM7" s="5">
+        <f>(AG7 + 2 * AH7 - AI7*(AJ7-1) -1) / AK7 + 1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AG8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH8" s="23"/>
+      <c r="AI8" s="23"/>
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="23"/>
+      <c r="AL8" s="23"/>
+      <c r="AM8" s="23"/>
+    </row>
+    <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="24"/>
+      <c r="AJ9" s="24"/>
+      <c r="AK9" s="24"/>
+      <c r="AL9" s="24"/>
+      <c r="AM9" s="24"/>
+    </row>
+    <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="I10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="22"/>
+      <c r="Q10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="22"/>
+      <c r="Y10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="22"/>
+      <c r="AG10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH10" s="21"/>
+      <c r="AI10" s="21"/>
+      <c r="AJ10" s="21"/>
+      <c r="AK10" s="21"/>
+      <c r="AL10" s="21"/>
+      <c r="AM10" s="22"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+      <c r="S11" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" t="s">
+        <v>3</v>
+      </c>
+      <c r="U11" t="s">
+        <v>4</v>
+      </c>
+      <c r="V11" t="s">
+        <v>22</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y11" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f>O12</f>
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f>G12/A12</f>
+        <v>2</v>
+      </c>
+      <c r="G12" s="11">
+        <f>E12*(A12-1) + D12 -2*B12</f>
+        <v>28</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="1">
+        <f>W12</f>
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <f>O12/I12</f>
+        <v>2</v>
+      </c>
+      <c r="O12" s="2">
+        <f>M12*(I12-1) + L12 -2*J12</f>
+        <v>14</v>
+      </c>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="1">
+        <f>AE12</f>
+        <v>4</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
+      <c r="U12">
+        <v>2</v>
+      </c>
+      <c r="V12">
+        <f>W12/Q12</f>
+        <v>1.75</v>
+      </c>
+      <c r="W12" s="2">
+        <f>U12*(Q12-1) + T12 -2*R12</f>
+        <v>7</v>
+      </c>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="15">
+        <f>AM12</f>
+        <v>2</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>4</v>
+      </c>
+      <c r="AC12">
+        <v>2</v>
+      </c>
+      <c r="AD12">
+        <f>AE12/Y12</f>
+        <v>2</v>
+      </c>
+      <c r="AE12" s="2">
+        <f>AC12*(Y12-1) + AB12 -2*Z12</f>
+        <v>4</v>
+      </c>
+      <c r="AF12" s="19"/>
+      <c r="AG12" s="1">
+        <f>AM5</f>
+        <v>1</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+      <c r="AJ12">
+        <v>2</v>
+      </c>
+      <c r="AK12">
+        <v>2</v>
+      </c>
+      <c r="AL12">
+        <f>AM12/AG12</f>
+        <v>2</v>
+      </c>
+      <c r="AM12" s="2">
+        <f>AK12*(AG12-1) + AJ12 -2*AH12</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="19"/>
+      <c r="I13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" t="s">
+        <v>3</v>
+      </c>
+      <c r="U13" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" t="s">
+        <v>22</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF13" s="19"/>
+      <c r="AG13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f>O14</f>
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4">
+        <f>G14/A14</f>
+        <v>2</v>
+      </c>
+      <c r="G14" s="12">
+        <f>E14*(A14-1) + D14 -2*B14</f>
+        <v>28</v>
+      </c>
+      <c r="H14" s="19"/>
+      <c r="I14" s="3">
+        <f>W14</f>
+        <v>7</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>4</v>
+      </c>
+      <c r="M14" s="4">
+        <v>2</v>
+      </c>
+      <c r="N14" s="4">
+        <f>O14/I14</f>
+        <v>2</v>
+      </c>
+      <c r="O14" s="5">
+        <f>M14*(I14-1) + L14 -2*J14</f>
+        <v>14</v>
+      </c>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="3">
+        <f>AE14</f>
+        <v>4</v>
+      </c>
+      <c r="R14" s="4">
+        <v>1</v>
+      </c>
+      <c r="S14" s="4">
+        <v>1</v>
+      </c>
+      <c r="T14" s="4">
+        <v>3</v>
+      </c>
+      <c r="U14" s="4">
+        <v>2</v>
+      </c>
+      <c r="V14" s="4">
+        <f>W14/Q14</f>
+        <v>1.75</v>
+      </c>
+      <c r="W14" s="5">
+        <f>U14*(Q14-1) + T14 -2*R14</f>
+        <v>7</v>
+      </c>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="16">
+        <f>AM14</f>
+        <v>2</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="4">
+        <v>4</v>
+      </c>
+      <c r="AC14" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="4">
+        <f>AE14/Y14</f>
+        <v>2</v>
+      </c>
+      <c r="AE14" s="5">
+        <f>AC14*(Y14-1) + AB14 -2*Z14</f>
+        <v>4</v>
+      </c>
+      <c r="AF14" s="19"/>
+      <c r="AG14" s="3">
+        <f>AM7</f>
+        <v>1</v>
+      </c>
+      <c r="AH14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK14" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL14" s="4">
+        <f>AM14/AG14</f>
+        <v>2</v>
+      </c>
+      <c r="AM14" s="5">
+        <f>AK14*(AG14-1) + AJ14 -2*AH14</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="P11:P14"/>
+    <mergeCell ref="X11:X14"/>
+    <mergeCell ref="AF11:AF14"/>
+    <mergeCell ref="AG8:AM8"/>
+    <mergeCell ref="AG9:AM9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="I10:O10"/>
+    <mergeCell ref="Q10:W10"/>
+    <mergeCell ref="Y10:AE10"/>
+    <mergeCell ref="AG10:AM10"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="Y3:AE3"/>
+    <mergeCell ref="AG3:AM3"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="X4:X7"/>
+    <mergeCell ref="AF4:AF7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mnist sort of working
</commit_message>
<xml_diff>
--- a/Convolutional network size calculator.xlsx
+++ b/Convolutional network size calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timva\Documents\GitHub\Sparse-recovery-of-IR-images-using-a-score-based-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9270EEE8-3857-40DE-A707-75E4FE0AA1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404A6366-C27C-4905-BB52-FE0E63B2748B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2B2DC737-34CF-420A-AF9A-B9F1BF30D588}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="31">
   <si>
     <t>Hin</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>28x28</t>
+  </si>
+  <si>
+    <t>Yang Song implementation</t>
   </si>
 </sst>
 </file>
@@ -5630,10 +5633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57EDBCC-9D54-4F0D-8FC8-82CD71FEE0A9}">
-  <dimension ref="A1:AM14"/>
+  <dimension ref="A1:AM28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AI19" sqref="AI19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6804,12 +6807,984 @@
         <v>2</v>
       </c>
     </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7"/>
+    </row>
+    <row r="16" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="7"/>
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="7"/>
+    </row>
+    <row r="17" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+      <c r="I17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="22"/>
+      <c r="Q17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="22"/>
+      <c r="Y17" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z17" s="21"/>
+      <c r="AA17" s="21"/>
+      <c r="AB17" s="21"/>
+      <c r="AC17" s="21"/>
+      <c r="AD17" s="21"/>
+      <c r="AE17" s="22"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" t="s">
+        <v>2</v>
+      </c>
+      <c r="T18" t="s">
+        <v>3</v>
+      </c>
+      <c r="U18" t="s">
+        <v>4</v>
+      </c>
+      <c r="V18" t="s">
+        <v>21</v>
+      </c>
+      <c r="W18" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="X18" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f>A19/G19</f>
+        <v>1.0769230769230769</v>
+      </c>
+      <c r="G19" s="2">
+        <f>(A19 + 2 * B19 - C19*(D19-1) -1) / E19 + 1</f>
+        <v>26</v>
+      </c>
+      <c r="H19" s="19"/>
+      <c r="I19" s="1">
+        <f>G19</f>
+        <v>26</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <f>I19/O19</f>
+        <v>2.08</v>
+      </c>
+      <c r="O19" s="2">
+        <f>(I19 + 2 * J19 - K19*(L19-1) -1) / M19 + 1</f>
+        <v>12.5</v>
+      </c>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="1">
+        <f>O19</f>
+        <v>12.5</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <f>Q19/W19</f>
+        <v>2.1739130434782608</v>
+      </c>
+      <c r="W19" s="13">
+        <f>(Q19 + 2 * R19 - S19*(T19-1) -1) / U19 + 1</f>
+        <v>5.75</v>
+      </c>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="1">
+        <f>W19</f>
+        <v>5.75</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>3</v>
+      </c>
+      <c r="AC19">
+        <v>2</v>
+      </c>
+      <c r="AD19">
+        <f>Y19/AE19</f>
+        <v>2.4210526315789473</v>
+      </c>
+      <c r="AE19" s="2">
+        <f>(Y19 + 2 * Z19 - AA19*(AB19-1) -1) / AC19 + 1</f>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R20" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" t="s">
+        <v>2</v>
+      </c>
+      <c r="T20" t="s">
+        <v>3</v>
+      </c>
+      <c r="U20" t="s">
+        <v>4</v>
+      </c>
+      <c r="V20" t="s">
+        <v>21</v>
+      </c>
+      <c r="W20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE20" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>28</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <f>A21/G21</f>
+        <v>1.0769230769230769</v>
+      </c>
+      <c r="G21" s="5">
+        <f>(A21 + 2 * B21 - C21*(D21-1) -1) / E21 + 1</f>
+        <v>26</v>
+      </c>
+      <c r="H21" s="19"/>
+      <c r="I21" s="3">
+        <f>G21</f>
+        <v>26</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
+      </c>
+      <c r="L21" s="4">
+        <v>3</v>
+      </c>
+      <c r="M21" s="4">
+        <v>2</v>
+      </c>
+      <c r="N21" s="4">
+        <f>I21/O21</f>
+        <v>2.08</v>
+      </c>
+      <c r="O21" s="5">
+        <f>(I21 + 2 * J21 - K21*(L21-1) -1) / M21 + 1</f>
+        <v>12.5</v>
+      </c>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="3">
+        <f>O21</f>
+        <v>12.5</v>
+      </c>
+      <c r="R21" s="4">
+        <v>0</v>
+      </c>
+      <c r="S21" s="4">
+        <v>1</v>
+      </c>
+      <c r="T21" s="4">
+        <v>3</v>
+      </c>
+      <c r="U21" s="4">
+        <v>2</v>
+      </c>
+      <c r="V21" s="4">
+        <f>Q21/W21</f>
+        <v>2.1739130434782608</v>
+      </c>
+      <c r="W21" s="14">
+        <f>(Q21 + 2 * R21 - S21*(T21-1) -1) / U21 + 1</f>
+        <v>5.75</v>
+      </c>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="3">
+        <f>W21</f>
+        <v>5.75</v>
+      </c>
+      <c r="Z21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC21" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="4">
+        <f>Y21/AE21</f>
+        <v>2.4210526315789473</v>
+      </c>
+      <c r="AE21" s="5">
+        <f>(Y21 + 2 * Z21 - AA21*(AB21-1) -1) / AC21 + 1</f>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Y22" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+      <c r="AD22" s="23"/>
+      <c r="AE22" s="23"/>
+    </row>
+    <row r="23" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z23" s="24"/>
+      <c r="AA23" s="24"/>
+      <c r="AB23" s="24"/>
+      <c r="AC23" s="24"/>
+      <c r="AD23" s="24"/>
+      <c r="AE23" s="24"/>
+    </row>
+    <row r="24" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
+      <c r="I24" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="22"/>
+      <c r="Q24" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="22"/>
+      <c r="Y24" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="21"/>
+      <c r="AC24" s="21"/>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="22"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" t="s">
+        <v>22</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P25" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q25" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="R25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S25" t="s">
+        <v>2</v>
+      </c>
+      <c r="T25" t="s">
+        <v>3</v>
+      </c>
+      <c r="U25" t="s">
+        <v>4</v>
+      </c>
+      <c r="V25" t="s">
+        <v>22</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X25" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f>O26</f>
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <f>G26/A26</f>
+        <v>2.0384615384615383</v>
+      </c>
+      <c r="G26" s="11">
+        <f>E26*(A26-1) + D26 -2*B26</f>
+        <v>53</v>
+      </c>
+      <c r="H26" s="19"/>
+      <c r="I26" s="1">
+        <f>W26</f>
+        <v>12.5</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <f>O26/I26</f>
+        <v>2.08</v>
+      </c>
+      <c r="O26" s="2">
+        <f>M26*(I26-1) + L26 -2*J26</f>
+        <v>26</v>
+      </c>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="15">
+        <f>AE26</f>
+        <v>5.75</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>3</v>
+      </c>
+      <c r="U26">
+        <v>2</v>
+      </c>
+      <c r="V26">
+        <f>W26/Q26</f>
+        <v>2.1739130434782608</v>
+      </c>
+      <c r="W26" s="2">
+        <f>U26*(Q26-1) + T26 -2*R26</f>
+        <v>12.5</v>
+      </c>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="1">
+        <f>AE19</f>
+        <v>2.375</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+      <c r="AB26">
+        <v>3</v>
+      </c>
+      <c r="AC26">
+        <v>2</v>
+      </c>
+      <c r="AD26">
+        <f>AE26/Y26</f>
+        <v>2.4210526315789473</v>
+      </c>
+      <c r="AE26" s="2">
+        <f>AC26*(Y26-1) + AB26 -2*Z26</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="19"/>
+      <c r="I27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>3</v>
+      </c>
+      <c r="M27" t="s">
+        <v>4</v>
+      </c>
+      <c r="N27" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="R27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S27" t="s">
+        <v>2</v>
+      </c>
+      <c r="T27" t="s">
+        <v>3</v>
+      </c>
+      <c r="U27" t="s">
+        <v>4</v>
+      </c>
+      <c r="V27" t="s">
+        <v>22</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <f>O28</f>
+        <v>26</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2</v>
+      </c>
+      <c r="F28" s="4">
+        <f>G28/A28</f>
+        <v>2.0384615384615383</v>
+      </c>
+      <c r="G28" s="12">
+        <f>E28*(A28-1) + D28 -2*B28</f>
+        <v>53</v>
+      </c>
+      <c r="H28" s="19"/>
+      <c r="I28" s="3">
+        <f>W28</f>
+        <v>12.5</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
+        <v>1</v>
+      </c>
+      <c r="L28" s="4">
+        <v>3</v>
+      </c>
+      <c r="M28" s="4">
+        <v>2</v>
+      </c>
+      <c r="N28" s="4">
+        <f>O28/I28</f>
+        <v>2.08</v>
+      </c>
+      <c r="O28" s="5">
+        <f>M28*(I28-1) + L28 -2*J28</f>
+        <v>26</v>
+      </c>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="16">
+        <f>AE28</f>
+        <v>5.75</v>
+      </c>
+      <c r="R28" s="4">
+        <v>0</v>
+      </c>
+      <c r="S28" s="4">
+        <v>1</v>
+      </c>
+      <c r="T28" s="4">
+        <v>3</v>
+      </c>
+      <c r="U28" s="4">
+        <v>2</v>
+      </c>
+      <c r="V28" s="4">
+        <f>W28/Q28</f>
+        <v>2.1739130434782608</v>
+      </c>
+      <c r="W28" s="5">
+        <f>U28*(Q28-1) + T28 -2*R28</f>
+        <v>12.5</v>
+      </c>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="3">
+        <f>AE21</f>
+        <v>2.375</v>
+      </c>
+      <c r="Z28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC28" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="4">
+        <f>AE28/Y28</f>
+        <v>2.4210526315789473</v>
+      </c>
+      <c r="AE28" s="5">
+        <f>AC28*(Y28-1) + AB28 -2*Z28</f>
+        <v>5.75</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="36">
+    <mergeCell ref="H25:H28"/>
+    <mergeCell ref="P25:P28"/>
+    <mergeCell ref="X25:X28"/>
+    <mergeCell ref="Y23:AE23"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="I24:O24"/>
+    <mergeCell ref="Q24:W24"/>
+    <mergeCell ref="Y24:AE24"/>
+    <mergeCell ref="Y17:AE17"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="P18:P21"/>
+    <mergeCell ref="X18:X21"/>
+    <mergeCell ref="Y22:AE22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="P11:P14"/>
     <mergeCell ref="X11:X14"/>
     <mergeCell ref="AF11:AF14"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="I17:O17"/>
+    <mergeCell ref="Q17:W17"/>
     <mergeCell ref="AG8:AM8"/>
     <mergeCell ref="AG9:AM9"/>
     <mergeCell ref="A10:G10"/>

</xml_diff>

<commit_message>
added calculation for new NN
</commit_message>
<xml_diff>
--- a/Convolutional network size calculator.xlsx
+++ b/Convolutional network size calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timva\Documents\GitHub\Sparse-recovery-of-IR-images-using-a-score-based-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olaf/Library/CloudStorage/OneDrive-DelftUniversityofTechnology/Master/Datacompression/Project/GithubClone/Sparse-recovery-of-IR-images-using-a-score-based-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404A6366-C27C-4905-BB52-FE0E63B2748B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B24397F-F1FA-6C41-978F-83439C9F3F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2B2DC737-34CF-420A-AF9A-B9F1BF30D588}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19800" activeTab="1" xr2:uid="{2B2DC737-34CF-420A-AF9A-B9F1BF30D588}"/>
   </bookViews>
   <sheets>
     <sheet name="NCSN" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="35">
   <si>
     <t>Hin</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>Yang Song implementation</t>
+  </si>
+  <si>
+    <t>512x512</t>
+  </si>
+  <si>
+    <t>Addapted Yang Song implementation</t>
+  </si>
+  <si>
+    <t>Conv 6</t>
+  </si>
+  <si>
+    <t>tConv 6</t>
   </si>
 </sst>
 </file>
@@ -346,7 +358,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,7 +374,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -684,17 +696,17 @@
       <selection activeCell="AM71" sqref="A58:AM71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="18"/>
       <c r="B1" s="6" t="s">
         <v>25</v>
@@ -704,7 +716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -712,7 +724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>8</v>
       </c>
@@ -750,7 +762,7 @@
       <c r="AD4" s="21"/>
       <c r="AE4" s="22"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
@@ -845,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>32</v>
       </c>
@@ -945,7 +957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>40</v>
       </c>
@@ -1134,7 +1146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="Y9" s="23" t="s">
         <v>15</v>
       </c>
@@ -1145,7 +1157,7 @@
       <c r="AD9" s="23"/>
       <c r="AE9" s="23"/>
     </row>
-    <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Y10" s="24" t="s">
         <v>16</v>
       </c>
@@ -1156,7 +1168,7 @@
       <c r="AD10" s="24"/>
       <c r="AE10" s="24"/>
     </row>
-    <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1206,7 @@
       <c r="AD11" s="21"/>
       <c r="AE11" s="22"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f>O13</f>
         <v>16</v>
@@ -1390,7 +1402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1479,7 +1491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <f>O15</f>
         <v>20</v>
@@ -1580,12 +1592,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:31" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H16" s="8"/>
       <c r="P16" s="8"/>
       <c r="X16" s="8"/>
     </row>
-    <row r="17" spans="1:39" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
@@ -1593,7 +1605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>8</v>
       </c>
@@ -1631,7 +1643,7 @@
       <c r="AD18" s="21"/>
       <c r="AE18" s="22"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>128</v>
       </c>
@@ -1826,7 +1838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>160</v>
       </c>
@@ -2015,7 +2027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="Y23" s="23" t="s">
         <v>15</v>
       </c>
@@ -2026,7 +2038,7 @@
       <c r="AD23" s="23"/>
       <c r="AE23" s="23"/>
     </row>
-    <row r="24" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Y24" s="24" t="s">
         <v>16</v>
       </c>
@@ -2037,7 +2049,7 @@
       <c r="AD24" s="24"/>
       <c r="AE24" s="24"/>
     </row>
-    <row r="25" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>8</v>
       </c>
@@ -2075,7 +2087,7 @@
       <c r="AD25" s="21"/>
       <c r="AE25" s="22"/>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <f>O27</f>
         <v>64</v>
@@ -2271,7 +2283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -2360,7 +2372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <f>O29</f>
         <v>80</v>
@@ -2461,12 +2473,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H30" s="8"/>
       <c r="P30" s="8"/>
       <c r="X30" s="8"/>
     </row>
-    <row r="31" spans="1:39" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
@@ -2477,7 +2489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>8</v>
       </c>
@@ -2524,7 +2536,7 @@
       <c r="AL32" s="21"/>
       <c r="AM32" s="22"/>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>0</v>
       </c>
@@ -2643,7 +2655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>128</v>
       </c>
@@ -2768,7 +2780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>6</v>
       </c>
@@ -2879,7 +2891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <v>160</v>
       </c>
@@ -3004,7 +3016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="AG37" s="23" t="s">
         <v>15</v>
       </c>
@@ -3015,7 +3027,7 @@
       <c r="AL37" s="23"/>
       <c r="AM37" s="23"/>
     </row>
-    <row r="38" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AG38" s="24" t="s">
         <v>16</v>
       </c>
@@ -3026,7 +3038,7 @@
       <c r="AL38" s="24"/>
       <c r="AM38" s="24"/>
     </row>
-    <row r="39" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>8</v>
       </c>
@@ -3073,7 +3085,7 @@
       <c r="AL39" s="21"/>
       <c r="AM39" s="22"/>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -3192,7 +3204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <f>O41</f>
         <v>64</v>
@@ -3318,7 +3330,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -3429,7 +3441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <f>O43</f>
         <v>80</v>
@@ -3555,12 +3567,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H44" s="8"/>
       <c r="P44" s="8"/>
       <c r="X44" s="8"/>
     </row>
-    <row r="45" spans="1:39" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>18</v>
       </c>
@@ -3571,7 +3583,7 @@
       <c r="P45" s="8"/>
       <c r="X45" s="8"/>
     </row>
-    <row r="46" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>8</v>
       </c>
@@ -3609,7 +3621,7 @@
       <c r="AD46" s="21"/>
       <c r="AE46" s="22"/>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>0</v>
       </c>
@@ -3704,7 +3716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>512</v>
       </c>
@@ -3804,7 +3816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>6</v>
       </c>
@@ -3893,7 +3905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" s="10">
         <v>640</v>
       </c>
@@ -3993,7 +4005,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="Y51" s="23" t="s">
         <v>15</v>
       </c>
@@ -4004,7 +4016,7 @@
       <c r="AD51" s="23"/>
       <c r="AE51" s="23"/>
     </row>
-    <row r="52" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Y52" s="24" t="s">
         <v>16</v>
       </c>
@@ -4015,7 +4027,7 @@
       <c r="AD52" s="24"/>
       <c r="AE52" s="24"/>
     </row>
-    <row r="53" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>8</v>
       </c>
@@ -4053,7 +4065,7 @@
       <c r="AD53" s="21"/>
       <c r="AE53" s="22"/>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -4148,7 +4160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <f>O55</f>
         <v>256</v>
@@ -4249,7 +4261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
@@ -4338,7 +4350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <f>O57</f>
         <v>320</v>
@@ -4439,12 +4451,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H58" s="8"/>
       <c r="P58" s="8"/>
       <c r="X58" s="8"/>
     </row>
-    <row r="59" spans="1:39" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:39" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>18</v>
       </c>
@@ -4458,7 +4470,7 @@
       <c r="P59" s="8"/>
       <c r="X59" s="8"/>
     </row>
-    <row r="60" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
         <v>8</v>
       </c>
@@ -4505,7 +4517,7 @@
       <c r="AL60" s="21"/>
       <c r="AM60" s="22"/>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>0</v>
       </c>
@@ -4624,7 +4636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>512</v>
       </c>
@@ -4749,7 +4761,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>6</v>
       </c>
@@ -4860,7 +4872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A64" s="10">
         <v>640</v>
       </c>
@@ -4985,7 +4997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
       <c r="AG65" s="23" t="s">
         <v>15</v>
       </c>
@@ -4996,7 +5008,7 @@
       <c r="AL65" s="23"/>
       <c r="AM65" s="23"/>
     </row>
-    <row r="66" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AG66" s="24" t="s">
         <v>16</v>
       </c>
@@ -5007,7 +5019,7 @@
       <c r="AL66" s="24"/>
       <c r="AM66" s="24"/>
     </row>
-    <row r="67" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>8</v>
       </c>
@@ -5054,7 +5066,7 @@
       <c r="AL67" s="21"/>
       <c r="AM67" s="22"/>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -5173,7 +5185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <f>O69</f>
         <v>256</v>
@@ -5299,7 +5311,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>6</v>
       </c>
@@ -5410,7 +5422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <f>O71</f>
         <v>320</v>
@@ -5538,42 +5550,42 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="X68:X71"/>
-    <mergeCell ref="AF68:AF71"/>
-    <mergeCell ref="I60:O60"/>
-    <mergeCell ref="P61:P64"/>
-    <mergeCell ref="I67:O67"/>
-    <mergeCell ref="P68:P71"/>
-    <mergeCell ref="AG65:AM65"/>
-    <mergeCell ref="AG66:AM66"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="Q67:W67"/>
-    <mergeCell ref="Y67:AE67"/>
-    <mergeCell ref="AG67:AM67"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="Q60:W60"/>
-    <mergeCell ref="Y60:AE60"/>
-    <mergeCell ref="AG60:AM60"/>
-    <mergeCell ref="H61:H64"/>
-    <mergeCell ref="X61:X64"/>
-    <mergeCell ref="AF61:AF64"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="I46:O46"/>
-    <mergeCell ref="Q46:W46"/>
-    <mergeCell ref="Y46:AE46"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="I53:O53"/>
-    <mergeCell ref="Q53:W53"/>
-    <mergeCell ref="Y53:AE53"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="P47:P50"/>
-    <mergeCell ref="X47:X50"/>
-    <mergeCell ref="Y51:AE51"/>
-    <mergeCell ref="Y52:AE52"/>
-    <mergeCell ref="X54:X57"/>
-    <mergeCell ref="P54:P57"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="P40:P43"/>
+    <mergeCell ref="X40:X43"/>
+    <mergeCell ref="AG32:AM32"/>
+    <mergeCell ref="AF33:AF36"/>
+    <mergeCell ref="AG37:AM37"/>
+    <mergeCell ref="AG38:AM38"/>
+    <mergeCell ref="AG39:AM39"/>
+    <mergeCell ref="AF40:AF43"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="I39:O39"/>
+    <mergeCell ref="Q39:W39"/>
+    <mergeCell ref="Y39:AE39"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="I32:O32"/>
+    <mergeCell ref="Q32:W32"/>
+    <mergeCell ref="Y32:AE32"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="P33:P36"/>
+    <mergeCell ref="X33:X36"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="P26:P29"/>
+    <mergeCell ref="X26:X29"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="P19:P22"/>
+    <mergeCell ref="X19:X22"/>
+    <mergeCell ref="Y24:AE24"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="I25:O25"/>
+    <mergeCell ref="Q25:W25"/>
+    <mergeCell ref="Y25:AE25"/>
+    <mergeCell ref="Y11:AE11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="P12:P15"/>
+    <mergeCell ref="X12:X15"/>
+    <mergeCell ref="Y23:AE23"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="I18:O18"/>
     <mergeCell ref="Q18:W18"/>
@@ -5590,42 +5602,42 @@
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="I11:O11"/>
     <mergeCell ref="Q11:W11"/>
-    <mergeCell ref="Y11:AE11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="P12:P15"/>
-    <mergeCell ref="X12:X15"/>
-    <mergeCell ref="Y23:AE23"/>
-    <mergeCell ref="Y24:AE24"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="I25:O25"/>
-    <mergeCell ref="Q25:W25"/>
-    <mergeCell ref="Y25:AE25"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="P26:P29"/>
-    <mergeCell ref="X26:X29"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="P19:P22"/>
-    <mergeCell ref="X19:X22"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="I39:O39"/>
-    <mergeCell ref="Q39:W39"/>
-    <mergeCell ref="Y39:AE39"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="I32:O32"/>
-    <mergeCell ref="Q32:W32"/>
-    <mergeCell ref="Y32:AE32"/>
-    <mergeCell ref="H33:H36"/>
-    <mergeCell ref="P33:P36"/>
-    <mergeCell ref="X33:X36"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="P40:P43"/>
-    <mergeCell ref="X40:X43"/>
-    <mergeCell ref="AG32:AM32"/>
-    <mergeCell ref="AF33:AF36"/>
-    <mergeCell ref="AG37:AM37"/>
-    <mergeCell ref="AG38:AM38"/>
-    <mergeCell ref="AG39:AM39"/>
-    <mergeCell ref="AF40:AF43"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="P47:P50"/>
+    <mergeCell ref="X47:X50"/>
+    <mergeCell ref="Y51:AE51"/>
+    <mergeCell ref="Y52:AE52"/>
+    <mergeCell ref="X54:X57"/>
+    <mergeCell ref="P54:P57"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="I46:O46"/>
+    <mergeCell ref="Q46:W46"/>
+    <mergeCell ref="Y46:AE46"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="I53:O53"/>
+    <mergeCell ref="Q53:W53"/>
+    <mergeCell ref="Y53:AE53"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="Q60:W60"/>
+    <mergeCell ref="Y60:AE60"/>
+    <mergeCell ref="AG60:AM60"/>
+    <mergeCell ref="H61:H64"/>
+    <mergeCell ref="X61:X64"/>
+    <mergeCell ref="AF61:AF64"/>
+    <mergeCell ref="AG65:AM65"/>
+    <mergeCell ref="AG66:AM66"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="Q67:W67"/>
+    <mergeCell ref="Y67:AE67"/>
+    <mergeCell ref="AG67:AM67"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="X68:X71"/>
+    <mergeCell ref="AF68:AF71"/>
+    <mergeCell ref="I60:O60"/>
+    <mergeCell ref="P61:P64"/>
+    <mergeCell ref="I67:O67"/>
+    <mergeCell ref="P68:P71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5633,15 +5645,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57EDBCC-9D54-4F0D-8FC8-82CD71FEE0A9}">
-  <dimension ref="A1:AM28"/>
+  <dimension ref="A1:AU42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -5682,7 +5694,7 @@
       <c r="AL1" s="7"/>
       <c r="AM1" s="7"/>
     </row>
-    <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -5729,7 +5741,7 @@
       <c r="AL2" s="7"/>
       <c r="AM2" s="7"/>
     </row>
-    <row r="3" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
@@ -5776,7 +5788,7 @@
       <c r="AL3" s="21"/>
       <c r="AM3" s="22"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -5895,7 +5907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>28</v>
       </c>
@@ -6020,7 +6032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -6131,7 +6143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>28</v>
       </c>
@@ -6256,7 +6268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="AG8" s="23" t="s">
         <v>15</v>
       </c>
@@ -6267,7 +6279,7 @@
       <c r="AL8" s="23"/>
       <c r="AM8" s="23"/>
     </row>
-    <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AG9" s="24" t="s">
         <v>16</v>
       </c>
@@ -6278,7 +6290,7 @@
       <c r="AL9" s="24"/>
       <c r="AM9" s="24"/>
     </row>
-    <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
@@ -6325,7 +6337,7 @@
       <c r="AL10" s="21"/>
       <c r="AM10" s="22"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -6444,7 +6456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f>O12</f>
         <v>14</v>
@@ -6570,7 +6582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -6681,7 +6693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <f>O14</f>
         <v>14</v>
@@ -6807,7 +6819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -6848,7 +6860,7 @@
       <c r="AL15" s="7"/>
       <c r="AM15" s="7"/>
     </row>
-    <row r="16" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
@@ -6895,7 +6907,7 @@
       <c r="AL16" s="7"/>
       <c r="AM16" s="7"/>
     </row>
-    <row r="17" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>8</v>
       </c>
@@ -6933,7 +6945,7 @@
       <c r="AD17" s="21"/>
       <c r="AE17" s="22"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -7028,7 +7040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>28</v>
       </c>
@@ -7128,7 +7140,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>6</v>
       </c>
@@ -7217,7 +7229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>28</v>
       </c>
@@ -7317,7 +7329,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="Y22" s="23" t="s">
         <v>15</v>
       </c>
@@ -7328,7 +7340,7 @@
       <c r="AD22" s="23"/>
       <c r="AE22" s="23"/>
     </row>
-    <row r="23" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Y23" s="24" t="s">
         <v>16</v>
       </c>
@@ -7339,7 +7351,7 @@
       <c r="AD23" s="24"/>
       <c r="AE23" s="24"/>
     </row>
-    <row r="24" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:47" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>8</v>
       </c>
@@ -7377,7 +7389,7 @@
       <c r="AD24" s="21"/>
       <c r="AE24" s="22"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -7472,7 +7484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <f>O26</f>
         <v>26</v>
@@ -7487,15 +7499,15 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26">
         <f>G26/A26</f>
-        <v>2.0384615384615383</v>
+        <v>1.0769230769230769</v>
       </c>
       <c r="G26" s="11">
         <f>E26*(A26-1) + D26 -2*B26</f>
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="1">
@@ -7573,7 +7585,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -7662,7 +7674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <f>O28</f>
         <v>26</v>
@@ -7677,15 +7689,15 @@
         <v>3</v>
       </c>
       <c r="E28" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4">
         <f>G28/A28</f>
-        <v>2.0384615384615383</v>
+        <v>1.0769230769230769</v>
       </c>
       <c r="G28" s="12">
         <f>E28*(A28-1) + D28 -2*B28</f>
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="3">
@@ -7763,8 +7775,1420 @@
         <v>5.75</v>
       </c>
     </row>
+    <row r="29" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
+      <c r="AC29" s="7"/>
+      <c r="AD29" s="7"/>
+      <c r="AE29" s="7"/>
+    </row>
+    <row r="30" spans="1:47" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="7"/>
+      <c r="AE30" s="7"/>
+    </row>
+    <row r="31" spans="1:47" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="22"/>
+      <c r="I31" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="22"/>
+      <c r="Q31" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="22"/>
+      <c r="Y31" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z31" s="21"/>
+      <c r="AA31" s="21"/>
+      <c r="AB31" s="21"/>
+      <c r="AC31" s="21"/>
+      <c r="AD31" s="21"/>
+      <c r="AE31" s="22"/>
+      <c r="AG31" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH31" s="21"/>
+      <c r="AI31" s="21"/>
+      <c r="AJ31" s="21"/>
+      <c r="AK31" s="21"/>
+      <c r="AL31" s="21"/>
+      <c r="AM31" s="22"/>
+      <c r="AO31" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP31" s="21"/>
+      <c r="AQ31" s="21"/>
+      <c r="AR31" s="21"/>
+      <c r="AS31" s="21"/>
+      <c r="AT31" s="21"/>
+      <c r="AU31" s="22"/>
+    </row>
+    <row r="32" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>2</v>
+      </c>
+      <c r="L32" t="s">
+        <v>3</v>
+      </c>
+      <c r="M32" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32" t="s">
+        <v>21</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P32" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R32" t="s">
+        <v>1</v>
+      </c>
+      <c r="S32" t="s">
+        <v>2</v>
+      </c>
+      <c r="T32" t="s">
+        <v>3</v>
+      </c>
+      <c r="U32" t="s">
+        <v>4</v>
+      </c>
+      <c r="V32" t="s">
+        <v>21</v>
+      </c>
+      <c r="W32" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="X32" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE32" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF32" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM32" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN32" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ32" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT32" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU32" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>512</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <f>A33/G33</f>
+        <v>1.003921568627451</v>
+      </c>
+      <c r="G33" s="2">
+        <f>(A33 + 2 * B33 - C33*(D33-1) -1) / E33 + 1</f>
+        <v>510</v>
+      </c>
+      <c r="H33" s="19"/>
+      <c r="I33" s="1">
+        <f>G33</f>
+        <v>510</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>3</v>
+      </c>
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="N33">
+        <f>I33/O33</f>
+        <v>2.0039292730844793</v>
+      </c>
+      <c r="O33" s="2">
+        <f>(I33 + 2 * J33 - K33*(L33-1) -1) / M33 + 1</f>
+        <v>254.5</v>
+      </c>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="1">
+        <f>O33</f>
+        <v>254.5</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>3</v>
+      </c>
+      <c r="U33">
+        <v>2</v>
+      </c>
+      <c r="V33">
+        <f>Q33/W33</f>
+        <v>2.0078895463510849</v>
+      </c>
+      <c r="W33" s="13">
+        <f>(Q33 + 2 * R33 - S33*(T33-1) -1) / U33 + 1</f>
+        <v>126.75</v>
+      </c>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="1">
+        <f>W33</f>
+        <v>126.75</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>1</v>
+      </c>
+      <c r="AB33">
+        <v>3</v>
+      </c>
+      <c r="AC33">
+        <v>2</v>
+      </c>
+      <c r="AD33">
+        <f>Y33/AE33</f>
+        <v>2.0159045725646125</v>
+      </c>
+      <c r="AE33" s="13">
+        <f>(Y33 + 2 * Z33 - AA33*(AB33-1) -1) / AC33 + 1</f>
+        <v>62.875</v>
+      </c>
+      <c r="AF33" s="19"/>
+      <c r="AG33" s="1">
+        <f>AE33</f>
+        <v>62.875</v>
+      </c>
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <v>1</v>
+      </c>
+      <c r="AJ33">
+        <v>3</v>
+      </c>
+      <c r="AK33">
+        <v>2</v>
+      </c>
+      <c r="AL33">
+        <f>AG33/AM33</f>
+        <v>2.0323232323232325</v>
+      </c>
+      <c r="AM33" s="13">
+        <f>(AG33 + 2 * AH33 - AI33*(AJ33-1) -1) / AK33 + 1</f>
+        <v>30.9375</v>
+      </c>
+      <c r="AN33" s="19"/>
+      <c r="AO33" s="1">
+        <f>AM33</f>
+        <v>30.9375</v>
+      </c>
+      <c r="AP33">
+        <v>0</v>
+      </c>
+      <c r="AQ33">
+        <v>1</v>
+      </c>
+      <c r="AR33">
+        <v>3</v>
+      </c>
+      <c r="AS33">
+        <v>2</v>
+      </c>
+      <c r="AT33">
+        <f>AO33/AU33</f>
+        <v>2.0668058455114822</v>
+      </c>
+      <c r="AU33" s="2">
+        <f>(AO33 + 2 * AP33 - AQ33*(AR33-1) -1) / AS33 + 1</f>
+        <v>14.96875</v>
+      </c>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="19"/>
+      <c r="I34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M34" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R34" t="s">
+        <v>1</v>
+      </c>
+      <c r="S34" t="s">
+        <v>2</v>
+      </c>
+      <c r="T34" t="s">
+        <v>3</v>
+      </c>
+      <c r="U34" t="s">
+        <v>4</v>
+      </c>
+      <c r="V34" t="s">
+        <v>21</v>
+      </c>
+      <c r="W34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF34" s="19"/>
+      <c r="AG34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN34" s="19"/>
+      <c r="AO34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ34" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT34" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU34" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>512</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35" s="4">
+        <v>3</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1</v>
+      </c>
+      <c r="F35" s="4">
+        <f>A35/G35</f>
+        <v>1.003921568627451</v>
+      </c>
+      <c r="G35" s="5">
+        <f>(A35 + 2 * B35 - C35*(D35-1) -1) / E35 + 1</f>
+        <v>510</v>
+      </c>
+      <c r="H35" s="19"/>
+      <c r="I35" s="3">
+        <f>G35</f>
+        <v>510</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4">
+        <v>1</v>
+      </c>
+      <c r="L35" s="4">
+        <v>3</v>
+      </c>
+      <c r="M35" s="4">
+        <v>2</v>
+      </c>
+      <c r="N35" s="4">
+        <f>I35/O35</f>
+        <v>2.0039292730844793</v>
+      </c>
+      <c r="O35" s="5">
+        <f>(I35 + 2 * J35 - K35*(L35-1) -1) / M35 + 1</f>
+        <v>254.5</v>
+      </c>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="3">
+        <f>O35</f>
+        <v>254.5</v>
+      </c>
+      <c r="R35" s="4">
+        <v>0</v>
+      </c>
+      <c r="S35" s="4">
+        <v>1</v>
+      </c>
+      <c r="T35" s="4">
+        <v>3</v>
+      </c>
+      <c r="U35" s="4">
+        <v>2</v>
+      </c>
+      <c r="V35" s="4">
+        <f>Q35/W35</f>
+        <v>2.0078895463510849</v>
+      </c>
+      <c r="W35" s="14">
+        <f>(Q35 + 2 * R35 - S35*(T35-1) -1) / U35 + 1</f>
+        <v>126.75</v>
+      </c>
+      <c r="X35" s="19"/>
+      <c r="Y35" s="3">
+        <f>W35</f>
+        <v>126.75</v>
+      </c>
+      <c r="Z35" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC35" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD35" s="4">
+        <f>Y35/AE35</f>
+        <v>2.0159045725646125</v>
+      </c>
+      <c r="AE35" s="14">
+        <f>(Y35 + 2 * Z35 - AA35*(AB35-1) -1) / AC35 + 1</f>
+        <v>62.875</v>
+      </c>
+      <c r="AF35" s="19"/>
+      <c r="AG35" s="3">
+        <f>AE35</f>
+        <v>62.875</v>
+      </c>
+      <c r="AH35" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="4">
+        <v>3</v>
+      </c>
+      <c r="AK35" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL35" s="4">
+        <f>AG35/AM35</f>
+        <v>2.0323232323232325</v>
+      </c>
+      <c r="AM35" s="14">
+        <f>(AG35 + 2 * AH35 - AI35*(AJ35-1) -1) / AK35 + 1</f>
+        <v>30.9375</v>
+      </c>
+      <c r="AN35" s="19"/>
+      <c r="AO35" s="3">
+        <f>AM35</f>
+        <v>30.9375</v>
+      </c>
+      <c r="AP35" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR35" s="4">
+        <v>3</v>
+      </c>
+      <c r="AS35" s="4">
+        <v>2</v>
+      </c>
+      <c r="AT35" s="4">
+        <f>AO35/AU35</f>
+        <v>2.0668058455114822</v>
+      </c>
+      <c r="AU35" s="5">
+        <f>(AO35 + 2 * AP35 - AQ35*(AR35-1) -1) / AS35 + 1</f>
+        <v>14.96875</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AO36" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP36" s="23"/>
+      <c r="AQ36" s="23"/>
+      <c r="AR36" s="23"/>
+      <c r="AS36" s="23"/>
+      <c r="AT36" s="23"/>
+      <c r="AU36" s="23"/>
+    </row>
+    <row r="37" spans="1:47" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AO37" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP37" s="24"/>
+      <c r="AQ37" s="24"/>
+      <c r="AR37" s="24"/>
+      <c r="AS37" s="24"/>
+      <c r="AT37" s="24"/>
+      <c r="AU37" s="24"/>
+    </row>
+    <row r="38" spans="1:47" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="22"/>
+      <c r="I38" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="22"/>
+      <c r="Q38" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="22"/>
+      <c r="Y38" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z38" s="21"/>
+      <c r="AA38" s="21"/>
+      <c r="AB38" s="21"/>
+      <c r="AC38" s="21"/>
+      <c r="AD38" s="21"/>
+      <c r="AE38" s="22"/>
+      <c r="AG38" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH38" s="21"/>
+      <c r="AI38" s="21"/>
+      <c r="AJ38" s="21"/>
+      <c r="AK38" s="21"/>
+      <c r="AL38" s="21"/>
+      <c r="AM38" s="22"/>
+      <c r="AO38" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP38" s="21"/>
+      <c r="AQ38" s="21"/>
+      <c r="AR38" s="21"/>
+      <c r="AS38" s="21"/>
+      <c r="AT38" s="21"/>
+      <c r="AU38" s="22"/>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
+        <v>2</v>
+      </c>
+      <c r="L39" t="s">
+        <v>3</v>
+      </c>
+      <c r="M39" t="s">
+        <v>4</v>
+      </c>
+      <c r="N39" t="s">
+        <v>22</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q39" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="R39" t="s">
+        <v>1</v>
+      </c>
+      <c r="S39" t="s">
+        <v>2</v>
+      </c>
+      <c r="T39" t="s">
+        <v>3</v>
+      </c>
+      <c r="U39" t="s">
+        <v>4</v>
+      </c>
+      <c r="V39" t="s">
+        <v>22</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y39" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG39" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH39" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK39" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AO39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP39" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ39" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS39" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f>O40</f>
+        <v>510</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <f>G40/A40</f>
+        <v>1.003921568627451</v>
+      </c>
+      <c r="G40" s="11">
+        <f>E40*(A40-1) + D40 -2*B40</f>
+        <v>512</v>
+      </c>
+      <c r="H40" s="19"/>
+      <c r="I40" s="1">
+        <f>W40</f>
+        <v>254.5</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>3</v>
+      </c>
+      <c r="M40">
+        <v>2</v>
+      </c>
+      <c r="N40">
+        <f>O40/I40</f>
+        <v>2.0039292730844793</v>
+      </c>
+      <c r="O40" s="2">
+        <f>M40*(I40-1) + L40 -2*J40</f>
+        <v>510</v>
+      </c>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="15">
+        <f>AE40</f>
+        <v>126.75</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="T40">
+        <v>3</v>
+      </c>
+      <c r="U40">
+        <v>2</v>
+      </c>
+      <c r="V40">
+        <f>W40/Q40</f>
+        <v>2.0078895463510849</v>
+      </c>
+      <c r="W40" s="2">
+        <f>U40*(Q40-1) + T40 -2*R40</f>
+        <v>254.5</v>
+      </c>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="15">
+        <f>AM40</f>
+        <v>62.875</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40">
+        <v>1</v>
+      </c>
+      <c r="AB40">
+        <v>3</v>
+      </c>
+      <c r="AC40">
+        <v>2</v>
+      </c>
+      <c r="AD40">
+        <f>AE40/Y40</f>
+        <v>2.0159045725646125</v>
+      </c>
+      <c r="AE40" s="2">
+        <f>AC40*(Y40-1) + AB40 -2*Z40</f>
+        <v>126.75</v>
+      </c>
+      <c r="AF40" s="19"/>
+      <c r="AG40" s="15">
+        <f>AU40</f>
+        <v>30.9375</v>
+      </c>
+      <c r="AH40">
+        <v>0</v>
+      </c>
+      <c r="AI40">
+        <v>1</v>
+      </c>
+      <c r="AJ40">
+        <v>3</v>
+      </c>
+      <c r="AK40">
+        <v>2</v>
+      </c>
+      <c r="AL40">
+        <f>AM40/AG40</f>
+        <v>2.0323232323232325</v>
+      </c>
+      <c r="AM40" s="2">
+        <f>AK40*(AG40-1) + AJ40 -2*AH40</f>
+        <v>62.875</v>
+      </c>
+      <c r="AN40" s="19"/>
+      <c r="AO40" s="1">
+        <f>AU33</f>
+        <v>14.96875</v>
+      </c>
+      <c r="AP40">
+        <v>0</v>
+      </c>
+      <c r="AQ40">
+        <v>1</v>
+      </c>
+      <c r="AR40">
+        <v>3</v>
+      </c>
+      <c r="AS40">
+        <v>2</v>
+      </c>
+      <c r="AT40">
+        <f>AU40/AO40</f>
+        <v>2.0668058455114822</v>
+      </c>
+      <c r="AU40" s="2">
+        <f>AS40*(AO40-1) + AR40 -2*AP40</f>
+        <v>30.9375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="19"/>
+      <c r="I41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41" t="s">
+        <v>1</v>
+      </c>
+      <c r="K41" t="s">
+        <v>2</v>
+      </c>
+      <c r="L41" t="s">
+        <v>3</v>
+      </c>
+      <c r="M41" t="s">
+        <v>4</v>
+      </c>
+      <c r="N41" t="s">
+        <v>22</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="R41" t="s">
+        <v>1</v>
+      </c>
+      <c r="S41" t="s">
+        <v>2</v>
+      </c>
+      <c r="T41" t="s">
+        <v>3</v>
+      </c>
+      <c r="U41" t="s">
+        <v>4</v>
+      </c>
+      <c r="V41" t="s">
+        <v>22</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X41" s="19"/>
+      <c r="Y41" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF41" s="19"/>
+      <c r="AG41" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN41" s="19"/>
+      <c r="AO41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ41" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS41" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU41" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <f>O42</f>
+        <v>510</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <v>3</v>
+      </c>
+      <c r="E42" s="4">
+        <v>1</v>
+      </c>
+      <c r="F42" s="4">
+        <f>G42/A42</f>
+        <v>1.003921568627451</v>
+      </c>
+      <c r="G42" s="12">
+        <f>E42*(A42-1) + D42 -2*B42</f>
+        <v>512</v>
+      </c>
+      <c r="H42" s="19"/>
+      <c r="I42" s="3">
+        <f>W42</f>
+        <v>254.5</v>
+      </c>
+      <c r="J42" s="4">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4">
+        <v>1</v>
+      </c>
+      <c r="L42" s="4">
+        <v>3</v>
+      </c>
+      <c r="M42" s="4">
+        <v>2</v>
+      </c>
+      <c r="N42" s="4">
+        <f>O42/I42</f>
+        <v>2.0039292730844793</v>
+      </c>
+      <c r="O42" s="5">
+        <f>M42*(I42-1) + L42 -2*J42</f>
+        <v>510</v>
+      </c>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="16">
+        <f>AE42</f>
+        <v>126.75</v>
+      </c>
+      <c r="R42" s="4">
+        <v>0</v>
+      </c>
+      <c r="S42" s="4">
+        <v>1</v>
+      </c>
+      <c r="T42" s="4">
+        <v>3</v>
+      </c>
+      <c r="U42" s="4">
+        <v>2</v>
+      </c>
+      <c r="V42" s="4">
+        <f>W42/Q42</f>
+        <v>2.0078895463510849</v>
+      </c>
+      <c r="W42" s="5">
+        <f>U42*(Q42-1) + T42 -2*R42</f>
+        <v>254.5</v>
+      </c>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="16">
+        <f>AM42</f>
+        <v>62.875</v>
+      </c>
+      <c r="Z42" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB42" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC42" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD42" s="4">
+        <f>AE42/Y42</f>
+        <v>2.0159045725646125</v>
+      </c>
+      <c r="AE42" s="5">
+        <f>AC42*(Y42-1) + AB42 -2*Z42</f>
+        <v>126.75</v>
+      </c>
+      <c r="AF42" s="19"/>
+      <c r="AG42" s="16">
+        <f>AU42</f>
+        <v>30.9375</v>
+      </c>
+      <c r="AH42" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ42" s="4">
+        <v>3</v>
+      </c>
+      <c r="AK42" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL42" s="4">
+        <f>AM42/AG42</f>
+        <v>2.0323232323232325</v>
+      </c>
+      <c r="AM42" s="5">
+        <f>AK42*(AG42-1) + AJ42 -2*AH42</f>
+        <v>62.875</v>
+      </c>
+      <c r="AN42" s="19"/>
+      <c r="AO42" s="3">
+        <f>AU35</f>
+        <v>14.96875</v>
+      </c>
+      <c r="AP42" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ42" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR42" s="4">
+        <v>3</v>
+      </c>
+      <c r="AS42" s="4">
+        <v>2</v>
+      </c>
+      <c r="AT42" s="4">
+        <f>AU42/AO42</f>
+        <v>2.0668058455114822</v>
+      </c>
+      <c r="AU42" s="5">
+        <f>AS42*(AO42-1) + AR42 -2*AP42</f>
+        <v>30.9375</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="60">
+    <mergeCell ref="AF39:AF42"/>
+    <mergeCell ref="AO31:AU31"/>
+    <mergeCell ref="AN32:AN35"/>
+    <mergeCell ref="AO36:AU36"/>
+    <mergeCell ref="AO37:AU37"/>
+    <mergeCell ref="AO38:AU38"/>
+    <mergeCell ref="AN39:AN42"/>
+    <mergeCell ref="AG31:AM31"/>
+    <mergeCell ref="AF32:AF35"/>
+    <mergeCell ref="AG38:AM38"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="I38:O38"/>
+    <mergeCell ref="Q38:W38"/>
+    <mergeCell ref="Y38:AE38"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="P39:P42"/>
+    <mergeCell ref="X39:X42"/>
+    <mergeCell ref="H32:H35"/>
+    <mergeCell ref="P32:P35"/>
+    <mergeCell ref="X32:X35"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="X4:X7"/>
+    <mergeCell ref="AF4:AF7"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="I31:O31"/>
+    <mergeCell ref="Q31:W31"/>
+    <mergeCell ref="Y31:AE31"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="Y3:AE3"/>
+    <mergeCell ref="AG3:AM3"/>
+    <mergeCell ref="AG8:AM8"/>
+    <mergeCell ref="AG9:AM9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="I10:O10"/>
+    <mergeCell ref="Q10:W10"/>
+    <mergeCell ref="Y10:AE10"/>
+    <mergeCell ref="AG10:AM10"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="P11:P14"/>
+    <mergeCell ref="X11:X14"/>
+    <mergeCell ref="AF11:AF14"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="I17:O17"/>
+    <mergeCell ref="Q17:W17"/>
+    <mergeCell ref="Y17:AE17"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="P18:P21"/>
+    <mergeCell ref="X18:X21"/>
+    <mergeCell ref="Y22:AE22"/>
     <mergeCell ref="H25:H28"/>
     <mergeCell ref="P25:P28"/>
     <mergeCell ref="X25:X28"/>
@@ -7773,34 +9197,6 @@
     <mergeCell ref="I24:O24"/>
     <mergeCell ref="Q24:W24"/>
     <mergeCell ref="Y24:AE24"/>
-    <mergeCell ref="Y17:AE17"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="P18:P21"/>
-    <mergeCell ref="X18:X21"/>
-    <mergeCell ref="Y22:AE22"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="P11:P14"/>
-    <mergeCell ref="X11:X14"/>
-    <mergeCell ref="AF11:AF14"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="I17:O17"/>
-    <mergeCell ref="Q17:W17"/>
-    <mergeCell ref="AG8:AM8"/>
-    <mergeCell ref="AG9:AM9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="I10:O10"/>
-    <mergeCell ref="Q10:W10"/>
-    <mergeCell ref="Y10:AE10"/>
-    <mergeCell ref="AG10:AM10"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="Y3:AE3"/>
-    <mergeCell ref="AG3:AM3"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="X4:X7"/>
-    <mergeCell ref="AF4:AF7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some changes to the excel
</commit_message>
<xml_diff>
--- a/Convolutional network size calculator.xlsx
+++ b/Convolutional network size calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olaf/Library/CloudStorage/OneDrive-DelftUniversityofTechnology/Master/Datacompression/Project/GithubClone/Sparse-recovery-of-IR-images-using-a-score-based-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B24397F-F1FA-6C41-978F-83439C9F3F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B067570B-B671-A243-8C2F-0CC36CABF55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19800" activeTab="1" xr2:uid="{2B2DC737-34CF-420A-AF9A-B9F1BF30D588}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="1" xr2:uid="{2B2DC737-34CF-420A-AF9A-B9F1BF30D588}"/>
   </bookViews>
   <sheets>
     <sheet name="NCSN" sheetId="1" r:id="rId1"/>
@@ -5647,8 +5647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57EDBCC-9D54-4F0D-8FC8-82CD71FEE0A9}">
   <dimension ref="A1:AU42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="V17" workbookViewId="0">
+      <selection activeCell="Z49" sqref="Z49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8048,7 +8048,7 @@
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -8064,16 +8064,16 @@
       </c>
       <c r="F33">
         <f>A33/G33</f>
-        <v>1.003921568627451</v>
+        <v>1.0158730158730158</v>
       </c>
       <c r="G33" s="2">
         <f>(A33 + 2 * B33 - C33*(D33-1) -1) / E33 + 1</f>
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="H33" s="19"/>
       <c r="I33" s="1">
         <f>G33</f>
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -8089,16 +8089,16 @@
       </c>
       <c r="N33">
         <f>I33/O33</f>
-        <v>2.0039292730844793</v>
+        <v>2.016</v>
       </c>
       <c r="O33" s="2">
         <f>(I33 + 2 * J33 - K33*(L33-1) -1) / M33 + 1</f>
-        <v>254.5</v>
+        <v>62.5</v>
       </c>
       <c r="P33" s="19"/>
       <c r="Q33" s="1">
         <f>O33</f>
-        <v>254.5</v>
+        <v>62.5</v>
       </c>
       <c r="R33">
         <v>0</v>
@@ -8114,16 +8114,16 @@
       </c>
       <c r="V33">
         <f>Q33/W33</f>
-        <v>2.0078895463510849</v>
+        <v>2.0325203252032522</v>
       </c>
       <c r="W33" s="13">
         <f>(Q33 + 2 * R33 - S33*(T33-1) -1) / U33 + 1</f>
-        <v>126.75</v>
+        <v>30.75</v>
       </c>
       <c r="X33" s="19"/>
       <c r="Y33" s="1">
         <f>W33</f>
-        <v>126.75</v>
+        <v>30.75</v>
       </c>
       <c r="Z33">
         <v>0</v>
@@ -8139,16 +8139,16 @@
       </c>
       <c r="AD33">
         <f>Y33/AE33</f>
-        <v>2.0159045725646125</v>
+        <v>2.0672268907563027</v>
       </c>
       <c r="AE33" s="13">
         <f>(Y33 + 2 * Z33 - AA33*(AB33-1) -1) / AC33 + 1</f>
-        <v>62.875</v>
+        <v>14.875</v>
       </c>
       <c r="AF33" s="19"/>
       <c r="AG33" s="1">
         <f>AE33</f>
-        <v>62.875</v>
+        <v>14.875</v>
       </c>
       <c r="AH33">
         <v>0</v>
@@ -8164,16 +8164,16 @@
       </c>
       <c r="AL33">
         <f>AG33/AM33</f>
-        <v>2.0323232323232325</v>
+        <v>2.144144144144144</v>
       </c>
       <c r="AM33" s="13">
         <f>(AG33 + 2 * AH33 - AI33*(AJ33-1) -1) / AK33 + 1</f>
-        <v>30.9375</v>
+        <v>6.9375</v>
       </c>
       <c r="AN33" s="19"/>
       <c r="AO33" s="1">
         <f>AM33</f>
-        <v>30.9375</v>
+        <v>6.9375</v>
       </c>
       <c r="AP33">
         <v>0</v>
@@ -8189,11 +8189,11 @@
       </c>
       <c r="AT33">
         <f>AO33/AU33</f>
-        <v>2.0668058455114822</v>
+        <v>2.3368421052631581</v>
       </c>
       <c r="AU33" s="2">
         <f>(AO33 + 2 * AP33 - AQ33*(AR33-1) -1) / AS33 + 1</f>
-        <v>14.96875</v>
+        <v>2.96875</v>
       </c>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.2">
@@ -8331,7 +8331,7 @@
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -8347,16 +8347,16 @@
       </c>
       <c r="F35" s="4">
         <f>A35/G35</f>
-        <v>1.003921568627451</v>
+        <v>1.0158730158730158</v>
       </c>
       <c r="G35" s="5">
         <f>(A35 + 2 * B35 - C35*(D35-1) -1) / E35 + 1</f>
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="H35" s="19"/>
       <c r="I35" s="3">
         <f>G35</f>
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="J35" s="4">
         <v>0</v>
@@ -8372,16 +8372,16 @@
       </c>
       <c r="N35" s="4">
         <f>I35/O35</f>
-        <v>2.0039292730844793</v>
+        <v>2.016</v>
       </c>
       <c r="O35" s="5">
         <f>(I35 + 2 * J35 - K35*(L35-1) -1) / M35 + 1</f>
-        <v>254.5</v>
+        <v>62.5</v>
       </c>
       <c r="P35" s="19"/>
       <c r="Q35" s="3">
         <f>O35</f>
-        <v>254.5</v>
+        <v>62.5</v>
       </c>
       <c r="R35" s="4">
         <v>0</v>
@@ -8397,16 +8397,16 @@
       </c>
       <c r="V35" s="4">
         <f>Q35/W35</f>
-        <v>2.0078895463510849</v>
+        <v>2.0325203252032522</v>
       </c>
       <c r="W35" s="14">
         <f>(Q35 + 2 * R35 - S35*(T35-1) -1) / U35 + 1</f>
-        <v>126.75</v>
+        <v>30.75</v>
       </c>
       <c r="X35" s="19"/>
       <c r="Y35" s="3">
         <f>W35</f>
-        <v>126.75</v>
+        <v>30.75</v>
       </c>
       <c r="Z35" s="4">
         <v>0</v>
@@ -8422,16 +8422,16 @@
       </c>
       <c r="AD35" s="4">
         <f>Y35/AE35</f>
-        <v>2.0159045725646125</v>
+        <v>2.0672268907563027</v>
       </c>
       <c r="AE35" s="14">
         <f>(Y35 + 2 * Z35 - AA35*(AB35-1) -1) / AC35 + 1</f>
-        <v>62.875</v>
+        <v>14.875</v>
       </c>
       <c r="AF35" s="19"/>
       <c r="AG35" s="3">
         <f>AE35</f>
-        <v>62.875</v>
+        <v>14.875</v>
       </c>
       <c r="AH35" s="4">
         <v>0</v>
@@ -8447,16 +8447,16 @@
       </c>
       <c r="AL35" s="4">
         <f>AG35/AM35</f>
-        <v>2.0323232323232325</v>
+        <v>2.144144144144144</v>
       </c>
       <c r="AM35" s="14">
         <f>(AG35 + 2 * AH35 - AI35*(AJ35-1) -1) / AK35 + 1</f>
-        <v>30.9375</v>
+        <v>6.9375</v>
       </c>
       <c r="AN35" s="19"/>
       <c r="AO35" s="3">
         <f>AM35</f>
-        <v>30.9375</v>
+        <v>6.9375</v>
       </c>
       <c r="AP35" s="4">
         <v>0</v>
@@ -8472,11 +8472,11 @@
       </c>
       <c r="AT35" s="4">
         <f>AO35/AU35</f>
-        <v>2.0668058455114822</v>
+        <v>2.3368421052631581</v>
       </c>
       <c r="AU35" s="5">
         <f>(AO35 + 2 * AP35 - AQ35*(AR35-1) -1) / AS35 + 1</f>
-        <v>14.96875</v>
+        <v>2.96875</v>
       </c>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.2">
@@ -8703,7 +8703,7 @@
     <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <f>O40</f>
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -8719,16 +8719,16 @@
       </c>
       <c r="F40">
         <f>G40/A40</f>
-        <v>1.003921568627451</v>
+        <v>1.0158730158730158</v>
       </c>
       <c r="G40" s="11">
         <f>E40*(A40-1) + D40 -2*B40</f>
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="H40" s="19"/>
       <c r="I40" s="1">
         <f>W40</f>
-        <v>254.5</v>
+        <v>62.5</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -8744,16 +8744,16 @@
       </c>
       <c r="N40">
         <f>O40/I40</f>
-        <v>2.0039292730844793</v>
+        <v>2.016</v>
       </c>
       <c r="O40" s="2">
         <f>M40*(I40-1) + L40 -2*J40</f>
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="P40" s="19"/>
       <c r="Q40" s="15">
         <f>AE40</f>
-        <v>126.75</v>
+        <v>30.75</v>
       </c>
       <c r="R40">
         <v>0</v>
@@ -8769,16 +8769,16 @@
       </c>
       <c r="V40">
         <f>W40/Q40</f>
-        <v>2.0078895463510849</v>
+        <v>2.0325203252032522</v>
       </c>
       <c r="W40" s="2">
         <f>U40*(Q40-1) + T40 -2*R40</f>
-        <v>254.5</v>
+        <v>62.5</v>
       </c>
       <c r="X40" s="19"/>
       <c r="Y40" s="15">
         <f>AM40</f>
-        <v>62.875</v>
+        <v>14.875</v>
       </c>
       <c r="Z40">
         <v>0</v>
@@ -8794,16 +8794,16 @@
       </c>
       <c r="AD40">
         <f>AE40/Y40</f>
-        <v>2.0159045725646125</v>
+        <v>2.0672268907563027</v>
       </c>
       <c r="AE40" s="2">
         <f>AC40*(Y40-1) + AB40 -2*Z40</f>
-        <v>126.75</v>
+        <v>30.75</v>
       </c>
       <c r="AF40" s="19"/>
       <c r="AG40" s="15">
         <f>AU40</f>
-        <v>30.9375</v>
+        <v>6.9375</v>
       </c>
       <c r="AH40">
         <v>0</v>
@@ -8819,16 +8819,16 @@
       </c>
       <c r="AL40">
         <f>AM40/AG40</f>
-        <v>2.0323232323232325</v>
+        <v>2.144144144144144</v>
       </c>
       <c r="AM40" s="2">
         <f>AK40*(AG40-1) + AJ40 -2*AH40</f>
-        <v>62.875</v>
+        <v>14.875</v>
       </c>
       <c r="AN40" s="19"/>
       <c r="AO40" s="1">
         <f>AU33</f>
-        <v>14.96875</v>
+        <v>2.96875</v>
       </c>
       <c r="AP40">
         <v>0</v>
@@ -8844,11 +8844,11 @@
       </c>
       <c r="AT40">
         <f>AU40/AO40</f>
-        <v>2.0668058455114822</v>
+        <v>2.3368421052631581</v>
       </c>
       <c r="AU40" s="2">
         <f>AS40*(AO40-1) + AR40 -2*AP40</f>
-        <v>30.9375</v>
+        <v>6.9375</v>
       </c>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.2">
@@ -8987,7 +8987,7 @@
     <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <f>O42</f>
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="B42" s="4">
         <v>0</v>
@@ -9003,16 +9003,16 @@
       </c>
       <c r="F42" s="4">
         <f>G42/A42</f>
-        <v>1.003921568627451</v>
+        <v>1.0158730158730158</v>
       </c>
       <c r="G42" s="12">
         <f>E42*(A42-1) + D42 -2*B42</f>
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="3">
         <f>W42</f>
-        <v>254.5</v>
+        <v>62.5</v>
       </c>
       <c r="J42" s="4">
         <v>0</v>
@@ -9028,16 +9028,16 @@
       </c>
       <c r="N42" s="4">
         <f>O42/I42</f>
-        <v>2.0039292730844793</v>
+        <v>2.016</v>
       </c>
       <c r="O42" s="5">
         <f>M42*(I42-1) + L42 -2*J42</f>
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="P42" s="19"/>
       <c r="Q42" s="16">
         <f>AE42</f>
-        <v>126.75</v>
+        <v>30.75</v>
       </c>
       <c r="R42" s="4">
         <v>0</v>
@@ -9053,16 +9053,16 @@
       </c>
       <c r="V42" s="4">
         <f>W42/Q42</f>
-        <v>2.0078895463510849</v>
+        <v>2.0325203252032522</v>
       </c>
       <c r="W42" s="5">
         <f>U42*(Q42-1) + T42 -2*R42</f>
-        <v>254.5</v>
+        <v>62.5</v>
       </c>
       <c r="X42" s="19"/>
       <c r="Y42" s="16">
         <f>AM42</f>
-        <v>62.875</v>
+        <v>14.875</v>
       </c>
       <c r="Z42" s="4">
         <v>0</v>
@@ -9078,16 +9078,16 @@
       </c>
       <c r="AD42" s="4">
         <f>AE42/Y42</f>
-        <v>2.0159045725646125</v>
+        <v>2.0672268907563027</v>
       </c>
       <c r="AE42" s="5">
         <f>AC42*(Y42-1) + AB42 -2*Z42</f>
-        <v>126.75</v>
+        <v>30.75</v>
       </c>
       <c r="AF42" s="19"/>
       <c r="AG42" s="16">
         <f>AU42</f>
-        <v>30.9375</v>
+        <v>6.9375</v>
       </c>
       <c r="AH42" s="4">
         <v>0</v>
@@ -9103,16 +9103,16 @@
       </c>
       <c r="AL42" s="4">
         <f>AM42/AG42</f>
-        <v>2.0323232323232325</v>
+        <v>2.144144144144144</v>
       </c>
       <c r="AM42" s="5">
         <f>AK42*(AG42-1) + AJ42 -2*AH42</f>
-        <v>62.875</v>
+        <v>14.875</v>
       </c>
       <c r="AN42" s="19"/>
       <c r="AO42" s="3">
         <f>AU35</f>
-        <v>14.96875</v>
+        <v>2.96875</v>
       </c>
       <c r="AP42" s="4">
         <v>0</v>
@@ -9128,11 +9128,11 @@
       </c>
       <c r="AT42" s="4">
         <f>AU42/AO42</f>
-        <v>2.0668058455114822</v>
+        <v>2.3368421052631581</v>
       </c>
       <c r="AU42" s="5">
         <f>AS42*(AO42-1) + AR42 -2*AP42</f>
-        <v>30.9375</v>
+        <v>6.9375</v>
       </c>
     </row>
   </sheetData>
@@ -9165,18 +9165,6 @@
     <mergeCell ref="I31:O31"/>
     <mergeCell ref="Q31:W31"/>
     <mergeCell ref="Y31:AE31"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="Y3:AE3"/>
-    <mergeCell ref="AG3:AM3"/>
-    <mergeCell ref="AG8:AM8"/>
-    <mergeCell ref="AG9:AM9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="I10:O10"/>
-    <mergeCell ref="Q10:W10"/>
-    <mergeCell ref="Y10:AE10"/>
-    <mergeCell ref="AG10:AM10"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="P11:P14"/>
     <mergeCell ref="X11:X14"/>
@@ -9188,15 +9176,27 @@
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="P18:P21"/>
     <mergeCell ref="X18:X21"/>
-    <mergeCell ref="Y22:AE22"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="Y3:AE3"/>
+    <mergeCell ref="AG3:AM3"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="I10:O10"/>
+    <mergeCell ref="Q10:W10"/>
+    <mergeCell ref="Y10:AE10"/>
+    <mergeCell ref="AG10:AM10"/>
     <mergeCell ref="H25:H28"/>
     <mergeCell ref="P25:P28"/>
     <mergeCell ref="X25:X28"/>
     <mergeCell ref="Y23:AE23"/>
+    <mergeCell ref="AG8:AM8"/>
+    <mergeCell ref="AG9:AM9"/>
     <mergeCell ref="A24:G24"/>
     <mergeCell ref="I24:O24"/>
     <mergeCell ref="Q24:W24"/>
     <mergeCell ref="Y24:AE24"/>
+    <mergeCell ref="Y22:AE22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>